<commit_message>
Updated with Fixed Assets Schedule
</commit_message>
<xml_diff>
--- a/Model.xlsx
+++ b/Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb7d91c61a0f33f7/Desktop/VS_Code/automated_financial_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3012" documentId="11_F25DC773A252ABDACC1048EDE15D42E05BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DC103C9-75CE-4196-A519-C06E362F883B}"/>
+  <xr:revisionPtr revIDLastSave="3312" documentId="11_F25DC773A252ABDACC1048EDE15D42E05BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B213C1C-36C9-4A35-BB98-98CB390188F4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,6 +46,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={603B89FB-D427-49C3-A4CD-6D873E5E11C3}</author>
+    <author>tc={09595CBA-CF47-4D47-9DA0-07CB4727C94B}</author>
+    <author>tc={EDAC56EA-9F4D-4961-8A42-58C0B17E2411}</author>
     <author>tc={87379581-145D-4850-A472-6CEEC181F31A}</author>
   </authors>
   <commentList>
@@ -57,7 +59,24 @@
     Adjustment to be made once the price has been adjusted.</t>
       </text>
     </comment>
-    <comment ref="F122" authorId="1" shapeId="0" xr:uid="{87379581-145D-4850-A472-6CEEC181F31A}">
+    <comment ref="C46" authorId="1" shapeId="0" xr:uid="{09595CBA-CF47-4D47-9DA0-07CB4727C94B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Check Management’s guidance for the average CAPEX for the next 5 years (heading - Capital Expenditure Plans)</t>
+      </text>
+    </comment>
+    <comment ref="K46" authorId="2" shapeId="0" xr:uid="{EDAC56EA-9F4D-4961-8A42-58C0B17E2411}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Mangement says it expects to spend a similar amount for 2025 as 2024, therefore, using 2024 as the base.
+</t>
+      </text>
+    </comment>
+    <comment ref="F122" authorId="3" shapeId="0" xr:uid="{87379581-145D-4850-A472-6CEEC181F31A}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -72,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="361">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1273,12 +1292,6 @@
     <t>Working Capital</t>
   </si>
   <si>
-    <t>Fixed Income Schedule</t>
-  </si>
-  <si>
-    <t>Fixed Income</t>
-  </si>
-  <si>
     <t>Days of Inventory</t>
   </si>
   <si>
@@ -1286,6 +1299,90 @@
   </si>
   <si>
     <t>Days of Payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warehouse Openings </t>
+  </si>
+  <si>
+    <t>CAPEX</t>
+  </si>
+  <si>
+    <t>Average CAPEX/Warehouse Openings</t>
+  </si>
+  <si>
+    <t>[Forecast] CAPEX (goes to CFI)</t>
+  </si>
+  <si>
+    <t>PPE Gross (notes: property and equipment - ending)</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Dispositions</t>
+  </si>
+  <si>
+    <t>Average PPE</t>
+  </si>
+  <si>
+    <t>Depreciation</t>
+  </si>
+  <si>
+    <t>Depreciation/Average PPE</t>
+  </si>
+  <si>
+    <t>[Forecast] Depreciation (goes to CFS)</t>
+  </si>
+  <si>
+    <t>PPE (beginning)</t>
+  </si>
+  <si>
+    <t>Add CAPEX</t>
+  </si>
+  <si>
+    <t>Less Depreciation</t>
+  </si>
+  <si>
+    <t>PPE Intermediate</t>
+  </si>
+  <si>
+    <t>Less: Derecognitions</t>
+  </si>
+  <si>
+    <t>Less: Impairments</t>
+  </si>
+  <si>
+    <t>PPE (ending) (goes to BS)</t>
+  </si>
+  <si>
+    <t>Average Dispositions</t>
+  </si>
+  <si>
+    <t>Average Depreciation Rate</t>
+  </si>
+  <si>
+    <t>Fixed Assets Schedule</t>
+  </si>
+  <si>
+    <t>Fixed Assets</t>
+  </si>
+  <si>
+    <t>Debt Schedule</t>
+  </si>
+  <si>
+    <t>Long Term Debt</t>
+  </si>
+  <si>
+    <t>CAPEX per warehouse</t>
+  </si>
+  <si>
+    <t>Inflation</t>
+  </si>
+  <si>
+    <t>Relocations</t>
+  </si>
+  <si>
+    <t>New builds</t>
   </si>
 </sst>
 </file>
@@ -1298,7 +1395,7 @@
     <numFmt numFmtId="165" formatCode="&quot;FY &quot;0"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1415,6 +1512,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1696,7 +1800,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2123,7 +2227,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2497,6 +2613,13 @@
   <threadedComment ref="K26" dT="2025-07-17T18:58:00.74" personId="{43DD08BC-4567-44A5-ADCC-A9C6F634F65D}" id="{603B89FB-D427-49C3-A4CD-6D873E5E11C3}">
     <text>Adjustment to be made once the price has been adjusted.</text>
   </threadedComment>
+  <threadedComment ref="C46" dT="2025-07-19T05:39:11.20" personId="{43DD08BC-4567-44A5-ADCC-A9C6F634F65D}" id="{09595CBA-CF47-4D47-9DA0-07CB4727C94B}">
+    <text>Check Management’s guidance for the average CAPEX for the next 5 years (heading - Capital Expenditure Plans)</text>
+  </threadedComment>
+  <threadedComment ref="K46" dT="2025-07-19T05:42:05.86" personId="{43DD08BC-4567-44A5-ADCC-A9C6F634F65D}" id="{EDAC56EA-9F4D-4961-8A42-58C0B17E2411}">
+    <text xml:space="preserve">Mangement says it expects to spend a similar amount for 2025 as 2024, therefore, using 2024 as the base.
+</text>
+  </threadedComment>
   <threadedComment ref="F122" dT="2025-07-13T19:39:44.27" personId="{43DD08BC-4567-44A5-ADCC-A9C6F634F65D}" id="{87379581-145D-4850-A472-6CEEC181F31A}">
     <text xml:space="preserve">Cash and Cash Equivalent from PY B.S.
 Others are being calculated, but should match the CCE of the B.S.
@@ -2507,10 +2630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:Q345"/>
+  <dimension ref="A2:Q381"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E348" sqref="E348"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -2692,7 +2815,7 @@
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
     </row>
-    <row r="12" spans="1:15" hidden="1" outlineLevel="1">
+    <row r="12" spans="1:15" outlineLevel="1">
       <c r="B12" s="182" t="s">
         <v>237</v>
       </c>
@@ -2725,7 +2848,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" outlineLevel="1">
+    <row r="13" spans="1:15" outlineLevel="1">
       <c r="B13" s="177"/>
       <c r="C13" s="178"/>
       <c r="D13" s="178"/>
@@ -2741,7 +2864,7 @@
       <c r="N13" s="194"/>
       <c r="O13" s="195"/>
     </row>
-    <row r="14" spans="1:15" hidden="1" outlineLevel="1">
+    <row r="14" spans="1:15" outlineLevel="1">
       <c r="B14" s="177" t="s">
         <v>5</v>
       </c>
@@ -2769,7 +2892,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" outlineLevel="1">
+    <row r="15" spans="1:15" outlineLevel="1">
       <c r="B15" s="177" t="s">
         <v>6</v>
       </c>
@@ -2797,7 +2920,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" outlineLevel="1">
+    <row r="16" spans="1:15" outlineLevel="1">
       <c r="B16" s="180" t="s">
         <v>7</v>
       </c>
@@ -2825,14 +2948,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="17" spans="2:15" outlineLevel="1">
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
     </row>
-    <row r="18" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="18" spans="2:15" outlineLevel="1">
       <c r="B18" s="182" t="s">
         <v>8</v>
       </c>
@@ -2865,7 +2988,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="19" spans="2:15" outlineLevel="1">
       <c r="B19" s="177"/>
       <c r="C19" s="178"/>
       <c r="D19" s="178"/>
@@ -2881,7 +3004,7 @@
       <c r="N19" s="194"/>
       <c r="O19" s="195"/>
     </row>
-    <row r="20" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="20" spans="2:15" outlineLevel="1">
       <c r="B20" s="177" t="s">
         <v>5</v>
       </c>
@@ -2909,7 +3032,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="21" spans="2:15" outlineLevel="1">
       <c r="B21" s="177" t="s">
         <v>6</v>
       </c>
@@ -2937,7 +3060,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="22" spans="2:15" outlineLevel="1">
       <c r="B22" s="180" t="s">
         <v>7</v>
       </c>
@@ -2965,21 +3088,21 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="23" spans="2:15" outlineLevel="1">
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
     </row>
-    <row r="24" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="24" spans="2:15" outlineLevel="1">
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
     </row>
-    <row r="25" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="25" spans="2:15" outlineLevel="1">
       <c r="B25" s="182" t="s">
         <v>203</v>
       </c>
@@ -2997,7 +3120,7 @@
       <c r="N25" s="197"/>
       <c r="O25" s="198"/>
     </row>
-    <row r="26" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="26" spans="2:15" outlineLevel="1">
       <c r="B26" s="192"/>
       <c r="C26" s="5" t="s">
         <v>281</v>
@@ -3032,7 +3155,7 @@
         <v>50.629233189982713</v>
       </c>
     </row>
-    <row r="27" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="27" spans="2:15" outlineLevel="1">
       <c r="B27" s="177"/>
       <c r="C27" s="178" t="s">
         <v>229</v>
@@ -3055,7 +3178,7 @@
       <c r="N27" s="204"/>
       <c r="O27" s="205"/>
     </row>
-    <row r="28" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="28" spans="2:15" outlineLevel="1">
       <c r="B28" s="177"/>
       <c r="C28" s="178" t="s">
         <v>309</v>
@@ -3078,7 +3201,7 @@
       <c r="N28" s="204"/>
       <c r="O28" s="205"/>
     </row>
-    <row r="29" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="29" spans="2:15" outlineLevel="1">
       <c r="B29" s="177"/>
       <c r="C29" s="178" t="s">
         <v>239</v>
@@ -3113,7 +3236,7 @@
         <v>8.2314720641173358E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="30" spans="2:15" outlineLevel="1">
       <c r="B30" s="180"/>
       <c r="C30" s="3" t="s">
         <v>282</v>
@@ -3136,14 +3259,14 @@
       <c r="N30" s="113"/>
       <c r="O30" s="196"/>
     </row>
-    <row r="31" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="31" spans="2:15" outlineLevel="1">
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
       <c r="O31" s="8"/>
     </row>
-    <row r="32" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="32" spans="2:15" outlineLevel="1">
       <c r="B32" s="182" t="s">
         <v>253</v>
       </c>
@@ -3161,7 +3284,7 @@
       <c r="N32" s="197"/>
       <c r="O32" s="198"/>
     </row>
-    <row r="33" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="33" spans="2:15" outlineLevel="1">
       <c r="B33" s="189"/>
       <c r="C33" s="178" t="s">
         <v>268</v>
@@ -3196,7 +3319,7 @@
         <v>5.4623415857288617E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="34" spans="2:15" outlineLevel="1">
       <c r="B34" s="188"/>
       <c r="C34" s="178" t="s">
         <v>283</v>
@@ -3218,7 +3341,7 @@
       <c r="N34" s="194"/>
       <c r="O34" s="195"/>
     </row>
-    <row r="35" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="35" spans="2:15" outlineLevel="1">
       <c r="B35" s="189"/>
       <c r="C35" s="5" t="s">
         <v>284</v>
@@ -3253,7 +3376,7 @@
         <v>1.2220039214117085E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="36" spans="2:15" outlineLevel="1">
       <c r="B36" s="190"/>
       <c r="C36" s="191" t="s">
         <v>283</v>
@@ -3275,7 +3398,7 @@
       <c r="N36" s="208"/>
       <c r="O36" s="210"/>
     </row>
-    <row r="37" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="37" spans="2:15" outlineLevel="1">
       <c r="B37" s="180"/>
       <c r="C37" s="3" t="s">
         <v>285</v>
@@ -3298,14 +3421,14 @@
       <c r="N37" s="113"/>
       <c r="O37" s="196"/>
     </row>
-    <row r="38" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="38" spans="2:15" outlineLevel="1">
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
       <c r="O38" s="8"/>
     </row>
-    <row r="39" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="39" spans="2:15" outlineLevel="1">
       <c r="B39" s="176" t="s">
         <v>16</v>
       </c>
@@ -3323,7 +3446,7 @@
       <c r="N39" s="105"/>
       <c r="O39" s="193"/>
     </row>
-    <row r="40" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="40" spans="2:15" outlineLevel="1">
       <c r="B40" s="180"/>
       <c r="C40" s="3" t="s">
         <v>304</v>
@@ -3361,7 +3484,7 @@
         <v>0.10860277351571095</v>
       </c>
     </row>
-    <row r="41" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="41" spans="2:15" outlineLevel="1">
       <c r="B41" s="200" t="s">
         <v>307</v>
       </c>
@@ -3379,7 +3502,7 @@
       <c r="N41" s="194"/>
       <c r="O41" s="195"/>
     </row>
-    <row r="42" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="42" spans="2:15" outlineLevel="1">
       <c r="B42" s="177"/>
       <c r="C42" s="178" t="s">
         <v>305</v>
@@ -3417,7 +3540,7 @@
         <v>8.3961180411072589E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:15" hidden="1" outlineLevel="1">
+    <row r="43" spans="2:15" outlineLevel="1">
       <c r="B43" s="180"/>
       <c r="C43" s="3" t="s">
         <v>306</v>
@@ -3440,19 +3563,125 @@
       <c r="N43" s="113"/>
       <c r="O43" s="196"/>
     </row>
-    <row r="44" spans="2:15" hidden="1" outlineLevel="1"/>
-    <row r="45" spans="2:15" hidden="1" outlineLevel="1"/>
-    <row r="46" spans="2:15" hidden="1" outlineLevel="1"/>
-    <row r="47" spans="2:15" hidden="1" outlineLevel="1"/>
-    <row r="48" spans="2:15" hidden="1" outlineLevel="1"/>
-    <row r="49" spans="1:15" hidden="1" outlineLevel="1"/>
-    <row r="50" spans="1:15" hidden="1" outlineLevel="1"/>
-    <row r="51" spans="1:15" hidden="1" outlineLevel="1"/>
-    <row r="52" spans="1:15" hidden="1" outlineLevel="1"/>
-    <row r="53" spans="1:15" hidden="1" outlineLevel="1"/>
-    <row r="54" spans="1:15" hidden="1" outlineLevel="1"/>
-    <row r="55" spans="1:15" hidden="1" outlineLevel="1"/>
-    <row r="56" spans="1:15" collapsed="1"/>
+    <row r="44" spans="2:15" outlineLevel="1">
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+    </row>
+    <row r="45" spans="2:15" outlineLevel="1">
+      <c r="B45" s="182" t="s">
+        <v>334</v>
+      </c>
+      <c r="C45" s="183"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="183"/>
+      <c r="F45" s="183"/>
+      <c r="G45" s="183"/>
+      <c r="H45" s="183"/>
+      <c r="I45" s="183"/>
+      <c r="J45" s="183"/>
+      <c r="K45" s="197"/>
+      <c r="L45" s="197"/>
+      <c r="M45" s="197"/>
+      <c r="N45" s="197"/>
+      <c r="O45" s="198"/>
+    </row>
+    <row r="46" spans="2:15" outlineLevel="1">
+      <c r="B46" s="177"/>
+      <c r="C46" s="178" t="s">
+        <v>357</v>
+      </c>
+      <c r="D46" s="178" t="s">
+        <v>209</v>
+      </c>
+      <c r="E46" s="178"/>
+      <c r="F46" s="178"/>
+      <c r="G46" s="178"/>
+      <c r="H46" s="178"/>
+      <c r="I46" s="178"/>
+      <c r="J46" s="178"/>
+      <c r="K46" s="219">
+        <f>J350*(1+$J$47)</f>
+        <v>165.66206896551725</v>
+      </c>
+      <c r="L46" s="219">
+        <f>K46*(1+$J$47)</f>
+        <v>168.97531034482759</v>
+      </c>
+      <c r="M46" s="219">
+        <f>L46*(1+$J$47)</f>
+        <v>172.35481655172416</v>
+      </c>
+      <c r="N46" s="219">
+        <f>M46*(1+$J$47)</f>
+        <v>175.80191288275864</v>
+      </c>
+      <c r="O46" s="220">
+        <f>N46*(1+$J$47)</f>
+        <v>179.31795114041381</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" outlineLevel="1">
+      <c r="B47" s="177"/>
+      <c r="C47" s="178" t="s">
+        <v>358</v>
+      </c>
+      <c r="D47" s="178" t="s">
+        <v>217</v>
+      </c>
+      <c r="E47" s="178"/>
+      <c r="F47" s="178"/>
+      <c r="G47" s="178"/>
+      <c r="H47" s="178"/>
+      <c r="I47" s="178"/>
+      <c r="J47" s="218">
+        <v>0.02</v>
+      </c>
+      <c r="K47" s="194"/>
+      <c r="L47" s="194"/>
+      <c r="M47" s="194"/>
+      <c r="N47" s="194"/>
+      <c r="O47" s="195"/>
+    </row>
+    <row r="48" spans="2:15" outlineLevel="1">
+      <c r="B48" s="180"/>
+      <c r="C48" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="113">
+        <v>3</v>
+      </c>
+      <c r="L48" s="113">
+        <v>2</v>
+      </c>
+      <c r="M48" s="113">
+        <v>2</v>
+      </c>
+      <c r="N48" s="113">
+        <v>2</v>
+      </c>
+      <c r="O48" s="196">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" outlineLevel="1"/>
+    <row r="50" spans="1:15" outlineLevel="1"/>
+    <row r="51" spans="1:15" outlineLevel="1"/>
+    <row r="52" spans="1:15" outlineLevel="1"/>
+    <row r="53" spans="1:15" outlineLevel="1"/>
+    <row r="54" spans="1:15" outlineLevel="1"/>
+    <row r="55" spans="1:15" outlineLevel="1"/>
     <row r="57" spans="1:15">
       <c r="A57" s="115" t="s">
         <v>9</v>
@@ -4356,23 +4585,23 @@
       <c r="J96" s="32">
         <v>7367</v>
       </c>
-      <c r="K96" s="175">
+      <c r="K96" s="29">
         <f>K75</f>
         <v>10246.441514687082</v>
       </c>
-      <c r="L96" s="8">
+      <c r="L96" s="29">
         <f t="shared" ref="L96:O96" si="12">L75</f>
         <v>11743.386236471852</v>
       </c>
-      <c r="M96" s="8">
+      <c r="M96" s="29">
         <f t="shared" si="12"/>
         <v>13323.465050991599</v>
       </c>
-      <c r="N96" s="8">
+      <c r="N96" s="29">
         <f t="shared" si="12"/>
         <v>14960.891043085576</v>
       </c>
-      <c r="O96" s="8">
+      <c r="O96" s="29">
         <f t="shared" si="12"/>
         <v>16794.672031055772</v>
       </c>
@@ -4396,11 +4625,26 @@
       <c r="J97" s="32">
         <v>2237</v>
       </c>
-      <c r="K97" s="8"/>
-      <c r="L97" s="8"/>
-      <c r="M97" s="8"/>
-      <c r="N97" s="8"/>
-      <c r="O97" s="8"/>
+      <c r="K97" s="29">
+        <f>-K371</f>
+        <v>2409.1035135608377</v>
+      </c>
+      <c r="L97" s="29">
+        <f>-L371</f>
+        <v>2601.0057317948117</v>
+      </c>
+      <c r="M97" s="29">
+        <f>-M371</f>
+        <v>2797.6916436195984</v>
+      </c>
+      <c r="N97" s="29">
+        <f>-N371</f>
+        <v>2999.2569229070127</v>
+      </c>
+      <c r="O97" s="29">
+        <f>-O371</f>
+        <v>3205.7991570063077</v>
+      </c>
     </row>
     <row r="98" spans="2:15" hidden="1" outlineLevel="1">
       <c r="C98" t="s">
@@ -4421,11 +4665,26 @@
       <c r="J98" s="32">
         <v>315</v>
       </c>
-      <c r="K98" s="8"/>
-      <c r="L98" s="8"/>
-      <c r="M98" s="8"/>
-      <c r="N98" s="8"/>
-      <c r="O98" s="8"/>
+      <c r="K98" s="29">
+        <f>AVERAGE(H98:J98)</f>
+        <v>368</v>
+      </c>
+      <c r="L98" s="29">
+        <f>K98</f>
+        <v>368</v>
+      </c>
+      <c r="M98" s="29">
+        <f t="shared" ref="M98:O98" si="13">L98</f>
+        <v>368</v>
+      </c>
+      <c r="N98" s="29">
+        <f t="shared" si="13"/>
+        <v>368</v>
+      </c>
+      <c r="O98" s="29">
+        <f t="shared" si="13"/>
+        <v>368</v>
+      </c>
     </row>
     <row r="99" spans="2:15" hidden="1" outlineLevel="1">
       <c r="C99" t="s">
@@ -4446,11 +4705,11 @@
       <c r="J99" s="32">
         <v>818</v>
       </c>
-      <c r="K99" s="8"/>
-      <c r="L99" s="8"/>
-      <c r="M99" s="8"/>
-      <c r="N99" s="8"/>
-      <c r="O99" s="8"/>
+      <c r="K99" s="29"/>
+      <c r="L99" s="29"/>
+      <c r="M99" s="29"/>
+      <c r="N99" s="29"/>
+      <c r="O99" s="29"/>
     </row>
     <row r="100" spans="2:15" hidden="1" outlineLevel="1">
       <c r="C100" t="s">
@@ -4471,11 +4730,11 @@
       <c r="J100" s="32">
         <v>-9</v>
       </c>
-      <c r="K100" s="8"/>
-      <c r="L100" s="8"/>
-      <c r="M100" s="8"/>
-      <c r="N100" s="8"/>
-      <c r="O100" s="8"/>
+      <c r="K100" s="29"/>
+      <c r="L100" s="29"/>
+      <c r="M100" s="29"/>
+      <c r="N100" s="29"/>
+      <c r="O100" s="29"/>
     </row>
     <row r="101" spans="2:15" hidden="1" outlineLevel="1">
       <c r="C101" t="s">
@@ -4486,11 +4745,11 @@
       <c r="H101" s="28"/>
       <c r="I101" s="28"/>
       <c r="J101" s="28"/>
-      <c r="K101" s="8"/>
-      <c r="L101" s="8"/>
-      <c r="M101" s="8"/>
-      <c r="N101" s="8"/>
-      <c r="O101" s="8"/>
+      <c r="K101" s="29"/>
+      <c r="L101" s="29"/>
+      <c r="M101" s="29"/>
+      <c r="N101" s="29"/>
+      <c r="O101" s="29"/>
     </row>
     <row r="102" spans="2:15" hidden="1" outlineLevel="1">
       <c r="C102" t="s">
@@ -4516,19 +4775,19 @@
         <v>-1416.8981655380121</v>
       </c>
       <c r="L102" s="29">
-        <f t="shared" ref="L102:O102" si="13">L327</f>
+        <f t="shared" ref="L102:O102" si="14">L327</f>
         <v>-1530.5711132903052</v>
       </c>
       <c r="M102" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-1707.2487330977783</v>
       </c>
       <c r="N102" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-1894.0647623913101</v>
       </c>
       <c r="O102" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-2105.1505351886917</v>
       </c>
     </row>
@@ -4556,19 +4815,19 @@
         <v>1475.7107992124074</v>
       </c>
       <c r="L103" s="29">
-        <f t="shared" ref="L103:O103" si="14">L328</f>
+        <f t="shared" ref="L103:O103" si="15">L328</f>
         <v>1594.1020856551186</v>
       </c>
       <c r="M103" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1778.1132431754122</v>
       </c>
       <c r="N103" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1972.6836354588741</v>
       </c>
       <c r="O103" s="29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2192.5311601812391</v>
       </c>
     </row>
@@ -4596,19 +4855,19 @@
         <v>1167.4769021301263</v>
       </c>
       <c r="L104" s="29">
-        <f t="shared" ref="L104:O104" si="15">L340</f>
+        <f t="shared" ref="L104:O104" si="16">L340</f>
         <v>1180.1876091418103</v>
       </c>
       <c r="M104" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1167.4086632739532</v>
       </c>
       <c r="N104" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1279.7296635687121</v>
       </c>
       <c r="O104" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1402.085148300102</v>
       </c>
     </row>
@@ -4640,24 +4899,24 @@
         <v>11339</v>
       </c>
       <c r="K105" s="31">
-        <f t="shared" ref="K105:O105" si="16">SUM(K102:K104,K96:K100)</f>
-        <v>11472.731050491602</v>
+        <f t="shared" ref="K105:O105" si="17">SUM(K102:K104,K96:K100)</f>
+        <v>14249.83456405244</v>
       </c>
       <c r="L105" s="31">
-        <f t="shared" si="16"/>
-        <v>12987.104817978476</v>
+        <f t="shared" si="17"/>
+        <v>15956.110549773288</v>
       </c>
       <c r="M105" s="31">
-        <f t="shared" si="16"/>
-        <v>14561.738224343186</v>
+        <f t="shared" si="17"/>
+        <v>17727.429867962783</v>
       </c>
       <c r="N105" s="31">
-        <f t="shared" si="16"/>
-        <v>16319.239579721852</v>
+        <f t="shared" si="17"/>
+        <v>19686.496502628866</v>
       </c>
       <c r="O105" s="31">
-        <f t="shared" si="16"/>
-        <v>18284.137804348422</v>
+        <f t="shared" si="17"/>
+        <v>21857.936961354731</v>
       </c>
     </row>
     <row r="106" spans="2:15" hidden="1" outlineLevel="1">
@@ -4706,11 +4965,26 @@
       <c r="J108" s="32">
         <v>-4710</v>
       </c>
-      <c r="K108" s="8"/>
-      <c r="L108" s="8"/>
-      <c r="M108" s="8"/>
-      <c r="N108" s="8"/>
-      <c r="O108" s="8"/>
+      <c r="K108" s="29">
+        <f>K353</f>
+        <v>4804.2000000000007</v>
+      </c>
+      <c r="L108" s="29">
+        <f t="shared" ref="L108:O108" si="18">L353</f>
+        <v>4900.2839999999997</v>
+      </c>
+      <c r="M108" s="29">
+        <f t="shared" si="18"/>
+        <v>4998.2896800000008</v>
+      </c>
+      <c r="N108" s="29">
+        <f t="shared" si="18"/>
+        <v>5098.2554736000011</v>
+      </c>
+      <c r="O108" s="29">
+        <f t="shared" si="18"/>
+        <v>5200.2205830720004</v>
+      </c>
     </row>
     <row r="109" spans="2:15" hidden="1" outlineLevel="1">
       <c r="C109" t="s">
@@ -4731,11 +5005,21 @@
       <c r="J109" s="32">
         <v>301</v>
       </c>
-      <c r="K109" s="8"/>
-      <c r="L109" s="8"/>
-      <c r="M109" s="8"/>
-      <c r="N109" s="8"/>
-      <c r="O109" s="8"/>
+      <c r="K109" s="29">
+        <v>0</v>
+      </c>
+      <c r="L109" s="29">
+        <v>0</v>
+      </c>
+      <c r="M109" s="29">
+        <v>0</v>
+      </c>
+      <c r="N109" s="29">
+        <v>0</v>
+      </c>
+      <c r="O109" s="29">
+        <v>0</v>
+      </c>
     </row>
     <row r="110" spans="2:15" hidden="1" outlineLevel="1">
       <c r="B110" s="5" t="s">
@@ -4765,24 +5049,24 @@
         <v>-4409</v>
       </c>
       <c r="K110" s="31">
-        <f t="shared" ref="K110:O110" si="17">SUM(K108:K109)</f>
-        <v>0</v>
+        <f t="shared" ref="K110:O110" si="19">SUM(K108:K109)</f>
+        <v>4804.2000000000007</v>
       </c>
       <c r="L110" s="31">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>4900.2839999999997</v>
       </c>
       <c r="M110" s="31">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>4998.2896800000008</v>
       </c>
       <c r="N110" s="31">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>5098.2554736000011</v>
       </c>
       <c r="O110" s="31">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>5200.2205830720004</v>
       </c>
     </row>
     <row r="111" spans="2:15" hidden="1" outlineLevel="1">
@@ -4963,23 +5247,23 @@
         <v>-10764</v>
       </c>
       <c r="K118" s="31">
-        <f t="shared" ref="K118:O118" si="18">SUM(K113:K117)</f>
+        <f t="shared" ref="K118:O118" si="20">SUM(K113:K117)</f>
         <v>0</v>
       </c>
       <c r="L118" s="31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M118" s="31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N118" s="31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O118" s="31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -5028,44 +5312,44 @@
       <c r="D121" s="5"/>
       <c r="E121" s="5"/>
       <c r="F121" s="30">
-        <f t="shared" ref="F121:K121" si="19">F105+F110+F118+F120</f>
+        <f t="shared" ref="F121:K121" si="21">F105+F110+F118+F120</f>
         <v>3893</v>
       </c>
       <c r="G121" s="30">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>-1019</v>
       </c>
       <c r="H121" s="30">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>-1055</v>
       </c>
       <c r="I121" s="30">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>3497</v>
       </c>
       <c r="J121" s="30">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>-3794</v>
       </c>
       <c r="K121" s="31">
-        <f t="shared" si="19"/>
-        <v>11472.731050491602</v>
+        <f t="shared" si="21"/>
+        <v>19054.034564052439</v>
       </c>
       <c r="L121" s="31">
-        <f t="shared" ref="L121:O121" si="20">L105+L110+L118+L120</f>
-        <v>12987.104817978476</v>
+        <f t="shared" ref="L121:O121" si="22">L105+L110+L118+L120</f>
+        <v>20856.394549773286</v>
       </c>
       <c r="M121" s="31">
-        <f t="shared" si="20"/>
-        <v>14561.738224343186</v>
+        <f t="shared" si="22"/>
+        <v>22725.719547962784</v>
       </c>
       <c r="N121" s="31">
-        <f t="shared" si="20"/>
-        <v>16319.239579721852</v>
+        <f t="shared" si="22"/>
+        <v>24784.751976228868</v>
       </c>
       <c r="O121" s="31">
-        <f t="shared" si="20"/>
-        <v>18284.137804348422</v>
+        <f t="shared" si="22"/>
+        <v>27058.157544426733</v>
       </c>
     </row>
     <row r="122" spans="2:15" hidden="1" outlineLevel="1">
@@ -5080,36 +5364,36 @@
         <v>12277</v>
       </c>
       <c r="H122" s="28">
-        <f t="shared" ref="H122:O122" si="21">G123</f>
+        <f t="shared" ref="H122:O122" si="23">G123</f>
         <v>11258</v>
       </c>
       <c r="I122" s="28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>10203</v>
       </c>
       <c r="J122" s="28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>13700</v>
       </c>
       <c r="K122" s="29">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>9906</v>
       </c>
       <c r="L122" s="29">
-        <f t="shared" si="21"/>
-        <v>21378.731050491602</v>
+        <f t="shared" si="23"/>
+        <v>28960.034564052439</v>
       </c>
       <c r="M122" s="29">
-        <f t="shared" si="21"/>
-        <v>34365.83586847008</v>
+        <f t="shared" si="23"/>
+        <v>49816.429113825725</v>
       </c>
       <c r="N122" s="29">
-        <f t="shared" si="21"/>
-        <v>48927.574092813265</v>
+        <f t="shared" si="23"/>
+        <v>72542.148661788509</v>
       </c>
       <c r="O122" s="29">
-        <f t="shared" si="21"/>
-        <v>65246.813672535121</v>
+        <f t="shared" si="23"/>
+        <v>97326.900638017381</v>
       </c>
     </row>
     <row r="123" spans="2:15" ht="15" hidden="1" outlineLevel="1" thickBot="1">
@@ -5120,44 +5404,44 @@
       <c r="D123" s="33"/>
       <c r="E123" s="33"/>
       <c r="F123" s="100">
-        <f t="shared" ref="F123:O123" si="22">F122+F121</f>
+        <f t="shared" ref="F123:O123" si="24">F122+F121</f>
         <v>12277</v>
       </c>
       <c r="G123" s="100">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>11258</v>
       </c>
       <c r="H123" s="100">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>10203</v>
       </c>
       <c r="I123" s="100">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>13700</v>
       </c>
       <c r="J123" s="100">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>9906</v>
       </c>
       <c r="K123" s="101">
-        <f t="shared" si="22"/>
-        <v>21378.731050491602</v>
+        <f t="shared" si="24"/>
+        <v>28960.034564052439</v>
       </c>
       <c r="L123" s="101">
-        <f t="shared" si="22"/>
-        <v>34365.83586847008</v>
+        <f t="shared" si="24"/>
+        <v>49816.429113825725</v>
       </c>
       <c r="M123" s="101">
-        <f t="shared" si="22"/>
-        <v>48927.574092813265</v>
+        <f t="shared" si="24"/>
+        <v>72542.148661788509</v>
       </c>
       <c r="N123" s="101">
-        <f t="shared" si="22"/>
-        <v>65246.813672535121</v>
+        <f t="shared" si="24"/>
+        <v>97326.900638017381</v>
       </c>
       <c r="O123" s="101">
-        <f t="shared" si="22"/>
-        <v>83530.951476883551</v>
+        <f t="shared" si="24"/>
+        <v>124385.05818244412</v>
       </c>
     </row>
     <row r="124" spans="2:15" ht="15" hidden="1" outlineLevel="1" thickTop="1">
@@ -5391,23 +5675,23 @@
       </c>
       <c r="K140" s="29">
         <f>K123</f>
-        <v>21378.731050491602</v>
+        <v>28960.034564052439</v>
       </c>
       <c r="L140" s="29">
-        <f t="shared" ref="L140:O140" si="23">L123</f>
-        <v>34365.83586847008</v>
+        <f t="shared" ref="L140:O140" si="25">L123</f>
+        <v>49816.429113825725</v>
       </c>
       <c r="M140" s="29">
-        <f t="shared" si="23"/>
-        <v>48927.574092813265</v>
+        <f t="shared" si="25"/>
+        <v>72542.148661788509</v>
       </c>
       <c r="N140" s="29">
-        <f t="shared" si="23"/>
-        <v>65246.813672535121</v>
+        <f t="shared" si="25"/>
+        <v>97326.900638017381</v>
       </c>
       <c r="O140" s="29">
-        <f t="shared" si="23"/>
-        <v>83530.951476883551</v>
+        <f t="shared" si="25"/>
+        <v>124385.05818244412</v>
       </c>
     </row>
     <row r="141" spans="1:17" hidden="1" outlineLevel="1">
@@ -5436,7 +5720,7 @@
       <c r="O141" s="29"/>
       <c r="Q141" s="157">
         <f>O145/K145-1</f>
-        <v>1.5382393689081248</v>
+        <v>1.9398247887029587</v>
       </c>
     </row>
     <row r="142" spans="1:17" hidden="1" outlineLevel="1">
@@ -5463,19 +5747,19 @@
         <v>2925.6898741668438</v>
       </c>
       <c r="L142" s="29">
-        <f t="shared" ref="L142:O142" si="24">L317</f>
+        <f t="shared" ref="L142:O142" si="26">L317</f>
         <v>3148.8756365197028</v>
       </c>
       <c r="M142" s="29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>3397.8242849776389</v>
       </c>
       <c r="N142" s="29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>3674.0141883864658</v>
       </c>
       <c r="O142" s="29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>3980.9843271692303</v>
       </c>
       <c r="Q142" s="160">
@@ -5507,19 +5791,19 @@
         <v>20063.898165538012</v>
       </c>
       <c r="L143" s="29">
-        <f t="shared" ref="L143:O143" si="25">L318</f>
+        <f t="shared" ref="L143:O143" si="27">L318</f>
         <v>21594.469278828317</v>
       </c>
       <c r="M143" s="29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>23301.718011926096</v>
       </c>
       <c r="N143" s="29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>25195.782774317406</v>
       </c>
       <c r="O143" s="29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>27300.933309506097</v>
       </c>
     </row>
@@ -5547,19 +5831,19 @@
         <v>1864.4418382231925</v>
       </c>
       <c r="L144" s="29">
-        <f t="shared" ref="L144:O144" si="26">L319</f>
+        <f t="shared" ref="L144:O144" si="28">L319</f>
         <v>2006.6704717843309</v>
       </c>
       <c r="M144" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>2165.3169092801268</v>
       </c>
       <c r="N144" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>2341.3232644844288</v>
       </c>
       <c r="O144" s="29">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>2536.9448082732247</v>
       </c>
       <c r="Q144" s="160">
@@ -5595,26 +5879,26 @@
         <v>34246</v>
       </c>
       <c r="K145" s="31">
-        <f t="shared" ref="K145:O145" si="27">SUM(K140:K144)</f>
-        <v>46232.760928419651</v>
+        <f t="shared" ref="K145:O145" si="29">SUM(K140:K144)</f>
+        <v>53814.064441980488</v>
       </c>
       <c r="L145" s="31">
-        <f t="shared" si="27"/>
-        <v>61115.851255602429</v>
+        <f t="shared" si="29"/>
+        <v>76566.444500958067</v>
       </c>
       <c r="M145" s="31">
-        <f t="shared" si="27"/>
-        <v>77792.43329899713</v>
+        <f t="shared" si="29"/>
+        <v>101407.00786797238</v>
       </c>
       <c r="N145" s="31">
-        <f t="shared" si="27"/>
-        <v>96457.933899723415</v>
+        <f t="shared" si="29"/>
+        <v>128538.02086520569</v>
       </c>
       <c r="O145" s="31">
-        <f t="shared" si="27"/>
-        <v>117349.81392183212</v>
-      </c>
-      <c r="Q145" s="212">
+        <f t="shared" si="29"/>
+        <v>158203.92062739268</v>
+      </c>
+      <c r="Q145" s="213">
         <f>O143/K143-1</f>
         <v>0.36069935584095525</v>
       </c>
@@ -5665,11 +5949,26 @@
       <c r="J148" s="32">
         <v>29032</v>
       </c>
-      <c r="K148" s="29"/>
-      <c r="L148" s="29"/>
-      <c r="M148" s="29"/>
-      <c r="N148" s="29"/>
-      <c r="O148" s="29"/>
+      <c r="K148" s="29">
+        <f>K376</f>
+        <v>31427.096486439161</v>
+      </c>
+      <c r="L148" s="29">
+        <f t="shared" ref="L148:O148" si="30">L376</f>
+        <v>33726.374754644348</v>
+      </c>
+      <c r="M148" s="29">
+        <f t="shared" si="30"/>
+        <v>35926.972791024753</v>
+      </c>
+      <c r="N148" s="29">
+        <f t="shared" si="30"/>
+        <v>38025.971341717741</v>
+      </c>
+      <c r="O148" s="29">
+        <f t="shared" si="30"/>
+        <v>40020.392767783429</v>
+      </c>
     </row>
     <row r="149" spans="2:17" hidden="1" outlineLevel="1">
       <c r="C149" t="s">
@@ -5690,11 +5989,26 @@
       <c r="J149" s="32">
         <v>2617</v>
       </c>
-      <c r="K149" s="29"/>
-      <c r="L149" s="29"/>
-      <c r="M149" s="29"/>
-      <c r="N149" s="29"/>
-      <c r="O149" s="29"/>
+      <c r="K149" s="29">
+        <f>AVERAGE(F149:J149)</f>
+        <v>2756.4</v>
+      </c>
+      <c r="L149" s="29">
+        <f t="shared" ref="L149:O149" si="31">K149</f>
+        <v>2756.4</v>
+      </c>
+      <c r="M149" s="29">
+        <f t="shared" si="31"/>
+        <v>2756.4</v>
+      </c>
+      <c r="N149" s="29">
+        <f t="shared" si="31"/>
+        <v>2756.4</v>
+      </c>
+      <c r="O149" s="29">
+        <f t="shared" si="31"/>
+        <v>2756.4</v>
+      </c>
     </row>
     <row r="150" spans="2:17" hidden="1" outlineLevel="1">
       <c r="C150" t="s">
@@ -5750,23 +6064,23 @@
       </c>
       <c r="K151" s="101">
         <f>SUM(K148:K150,K145)</f>
-        <v>46232.760928419651</v>
+        <v>87997.56092841964</v>
       </c>
       <c r="L151" s="101">
         <f>SUM(L148:L150,L145)</f>
-        <v>61115.851255602429</v>
+        <v>113049.21925560242</v>
       </c>
       <c r="M151" s="101">
         <f>SUM(M148:M150,M145)</f>
-        <v>77792.43329899713</v>
+        <v>140090.38065899714</v>
       </c>
       <c r="N151" s="101">
         <f>SUM(N148:N150,N145)</f>
-        <v>96457.933899723415</v>
+        <v>169320.39220692342</v>
       </c>
       <c r="O151" s="101">
         <f>SUM(O148:O150,O145)</f>
-        <v>117349.81392183212</v>
+        <v>200980.71339517611</v>
       </c>
     </row>
     <row r="152" spans="2:17" ht="15" hidden="1" outlineLevel="1" thickTop="1">
@@ -5820,19 +6134,19 @@
         <v>20896.710799212407</v>
       </c>
       <c r="L154" s="29">
-        <f t="shared" ref="L154:O154" si="28">L321</f>
+        <f t="shared" ref="L154:O154" si="32">L321</f>
         <v>22490.812884867526</v>
       </c>
       <c r="M154" s="29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>24268.926128042938</v>
       </c>
       <c r="N154" s="29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>26241.609763501812</v>
       </c>
       <c r="O154" s="29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>28434.140923683051</v>
       </c>
     </row>
@@ -5860,19 +6174,19 @@
         <v>5188.6909559295627</v>
       </c>
       <c r="L155" s="29">
-        <f t="shared" ref="L155:O155" si="29">L304</f>
+        <f t="shared" ref="L155:O155" si="33">L304</f>
         <v>5486.5437099844812</v>
       </c>
       <c r="M155" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>5814.5965256484733</v>
       </c>
       <c r="N155" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>6172.9287460185678</v>
       </c>
       <c r="O155" s="29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>6564.833785350057</v>
       </c>
     </row>
@@ -5900,19 +6214,19 @@
         <v>2778.1493779941638</v>
       </c>
       <c r="L156" s="29">
-        <f t="shared" ref="L156:O156" si="30">L276</f>
+        <f t="shared" ref="L156:O156" si="34">L276</f>
         <v>3153.9523052301415</v>
       </c>
       <c r="M156" s="29">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>3566.4548327032235</v>
       </c>
       <c r="N156" s="29">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>4020.0445687305178</v>
       </c>
       <c r="O156" s="29">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>4519.7214969497145</v>
       </c>
     </row>
@@ -5940,19 +6254,19 @@
         <v>2798.6149845375976</v>
       </c>
       <c r="L157" s="29">
-        <f t="shared" ref="L157:O157" si="31">L234</f>
+        <f t="shared" ref="L157:O157" si="35">L234</f>
         <v>3161.1957867254223</v>
       </c>
       <c r="M157" s="29">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>3427.4813457290124</v>
       </c>
       <c r="N157" s="29">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>3717.1511328406177</v>
       </c>
       <c r="O157" s="29">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>4029.6636507588128</v>
       </c>
     </row>
@@ -6005,19 +6319,19 @@
         <v>6677.1532960588384</v>
       </c>
       <c r="L159" s="29">
-        <f t="shared" ref="L159:O159" si="32">L325</f>
+        <f t="shared" ref="L159:O159" si="36">L325</f>
         <v>7186.5188176359252</v>
       </c>
       <c r="M159" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>7754.6816647229462</v>
       </c>
       <c r="N159" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>8385.0158433957931</v>
       </c>
       <c r="O159" s="29">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>9085.5981887985745</v>
       </c>
     </row>
@@ -6049,23 +6363,23 @@
         <v>35361</v>
       </c>
       <c r="K160" s="31">
-        <f t="shared" ref="K160:O160" si="33">SUM(K154:K159)</f>
+        <f t="shared" ref="K160:O160" si="37">SUM(K154:K159)</f>
         <v>38339.31941373257</v>
       </c>
       <c r="L160" s="31">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>41479.023504443496</v>
       </c>
       <c r="M160" s="31">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>44832.140496846594</v>
       </c>
       <c r="N160" s="31">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>48536.750054487311</v>
       </c>
       <c r="O160" s="31">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>52633.95804554021</v>
       </c>
     </row>
@@ -6140,11 +6454,26 @@
       <c r="J164" s="32">
         <v>2375</v>
       </c>
-      <c r="K164" s="29"/>
-      <c r="L164" s="29"/>
-      <c r="M164" s="29"/>
-      <c r="N164" s="29"/>
-      <c r="O164" s="29"/>
+      <c r="K164" s="29">
+        <f>AVERAGE(F164:J164)</f>
+        <v>2496.6</v>
+      </c>
+      <c r="L164" s="29">
+        <f>K164</f>
+        <v>2496.6</v>
+      </c>
+      <c r="M164" s="29">
+        <f t="shared" ref="M164:O164" si="38">L164</f>
+        <v>2496.6</v>
+      </c>
+      <c r="N164" s="29">
+        <f t="shared" si="38"/>
+        <v>2496.6</v>
+      </c>
+      <c r="O164" s="29">
+        <f t="shared" si="38"/>
+        <v>2496.6</v>
+      </c>
     </row>
     <row r="165" spans="2:15" hidden="1" outlineLevel="1">
       <c r="C165" t="s">
@@ -6200,23 +6529,23 @@
       </c>
       <c r="K166" s="31">
         <f>SUM(K163:K165,K160)</f>
-        <v>38339.31941373257</v>
+        <v>40835.919413732569</v>
       </c>
       <c r="L166" s="31">
         <f>SUM(L163:L165,L160)</f>
-        <v>41479.023504443496</v>
+        <v>43975.623504443494</v>
       </c>
       <c r="M166" s="31">
         <f>SUM(M163:M165,M160)</f>
-        <v>44832.140496846594</v>
+        <v>47328.740496846593</v>
       </c>
       <c r="N166" s="31">
         <f>SUM(N163:N165,N160)</f>
-        <v>48536.750054487311</v>
+        <v>51033.35005448731</v>
       </c>
       <c r="O166" s="31">
         <f>SUM(O163:O165,O160)</f>
-        <v>52633.95804554021</v>
+        <v>55130.558045540209</v>
       </c>
     </row>
     <row r="167" spans="2:15" hidden="1" outlineLevel="1">
@@ -6357,31 +6686,31 @@
         <v>20642</v>
       </c>
       <c r="I172" s="30">
-        <f t="shared" ref="I172:O172" si="34">SUM(I169:I171)</f>
+        <f t="shared" ref="I172:O172" si="39">SUM(I169:I171)</f>
         <v>25058</v>
       </c>
       <c r="J172" s="30">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>23622</v>
       </c>
       <c r="K172" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>27865.441514687082</v>
       </c>
       <c r="L172" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>39608.827751158933</v>
       </c>
       <c r="M172" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>52932.292802150536</v>
       </c>
       <c r="N172" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>67893.183845236112</v>
       </c>
       <c r="O172" s="31">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>84687.855876291884</v>
       </c>
     </row>
@@ -6422,39 +6751,39 @@
         <v>18705</v>
       </c>
       <c r="G174" s="30">
-        <f t="shared" ref="G174:O174" si="35">SUM(G172:G173)</f>
+        <f t="shared" ref="G174:O174" si="40">SUM(G172:G173)</f>
         <v>18078</v>
       </c>
       <c r="H174" s="30">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>20647</v>
       </c>
       <c r="I174" s="30">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>25058</v>
       </c>
       <c r="J174" s="30">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>23622</v>
       </c>
       <c r="K174" s="31">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>27865.441514687082</v>
       </c>
       <c r="L174" s="31">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>39608.827751158933</v>
       </c>
       <c r="M174" s="31">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>52932.292802150536</v>
       </c>
       <c r="N174" s="31">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>67893.183845236112</v>
       </c>
       <c r="O174" s="31">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>84687.855876291884</v>
       </c>
     </row>
@@ -6470,40 +6799,40 @@
         <v>55556</v>
       </c>
       <c r="G175" s="100">
-        <f t="shared" ref="G175:O175" si="36">SUM(G174,G166)</f>
+        <f t="shared" ref="G175:O175" si="41">SUM(G174,G166)</f>
         <v>59268</v>
       </c>
       <c r="H175" s="100">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>64166</v>
       </c>
       <c r="I175" s="100">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>68994</v>
       </c>
       <c r="J175" s="100">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>69831</v>
       </c>
       <c r="K175" s="101">
-        <f t="shared" si="36"/>
-        <v>66204.760928419651</v>
+        <f t="shared" si="41"/>
+        <v>68701.360928419657</v>
       </c>
       <c r="L175" s="101">
-        <f t="shared" si="36"/>
-        <v>81087.851255602436</v>
+        <f t="shared" si="41"/>
+        <v>83584.451255602427</v>
       </c>
       <c r="M175" s="101">
-        <f t="shared" si="36"/>
-        <v>97764.43329899713</v>
+        <f t="shared" si="41"/>
+        <v>100261.03329899712</v>
       </c>
       <c r="N175" s="101">
-        <f t="shared" si="36"/>
-        <v>116429.93389972343</v>
+        <f t="shared" si="41"/>
+        <v>118926.53389972342</v>
       </c>
       <c r="O175" s="101">
-        <f t="shared" si="36"/>
-        <v>137321.8139218321</v>
+        <f t="shared" si="41"/>
+        <v>139818.41392183211</v>
       </c>
     </row>
     <row r="176" spans="2:15" ht="15" hidden="1" outlineLevel="1" thickTop="1"/>
@@ -6568,27 +6897,27 @@
       <c r="C191" s="3"/>
       <c r="D191" s="3"/>
       <c r="E191" s="4">
-        <f t="shared" ref="E191:J191" si="37">F191-1</f>
+        <f t="shared" ref="E191:J191" si="42">F191-1</f>
         <v>2019</v>
       </c>
       <c r="F191" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>2020</v>
       </c>
       <c r="G191" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>2021</v>
       </c>
       <c r="H191" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>2022</v>
       </c>
       <c r="I191" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>2023</v>
       </c>
       <c r="J191" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>2024</v>
       </c>
       <c r="K191" s="7">
@@ -6683,27 +7012,27 @@
         <v>52</v>
       </c>
       <c r="E194" s="106">
-        <f t="shared" ref="E194:J194" si="38">SUM(E192:E193)</f>
+        <f t="shared" ref="E194:J194" si="43">SUM(E192:E193)</f>
         <v>74700</v>
       </c>
       <c r="F194" s="106">
-        <f t="shared" si="38"/>
+        <f t="shared" si="43"/>
         <v>80700</v>
       </c>
       <c r="G194" s="106">
-        <f t="shared" si="38"/>
+        <f t="shared" si="43"/>
         <v>87300</v>
       </c>
       <c r="H194" s="106">
-        <f t="shared" si="38"/>
+        <f t="shared" si="43"/>
         <v>94900</v>
       </c>
       <c r="I194" s="106">
-        <f t="shared" si="38"/>
+        <f t="shared" si="43"/>
         <v>103300</v>
       </c>
       <c r="J194" s="106">
-        <f t="shared" si="38"/>
+        <f t="shared" si="43"/>
         <v>111600</v>
       </c>
       <c r="K194" s="105"/>
@@ -6822,19 +7151,19 @@
         <v>140</v>
       </c>
       <c r="G199" s="28">
-        <f t="shared" ref="G199:J199" si="39">G198-F198</f>
+        <f t="shared" ref="G199:J199" si="44">G198-F198</f>
         <v>191</v>
       </c>
       <c r="H199" s="28">
-        <f t="shared" si="39"/>
+        <f t="shared" si="44"/>
         <v>132</v>
       </c>
       <c r="I199" s="28">
-        <f t="shared" si="39"/>
+        <f t="shared" si="44"/>
         <v>163</v>
       </c>
       <c r="J199" s="28">
-        <f t="shared" si="39"/>
+        <f t="shared" si="44"/>
         <v>164</v>
       </c>
       <c r="K199" s="8"/>
@@ -6892,19 +7221,19 @@
         <v>3681</v>
       </c>
       <c r="G202" s="107">
-        <f t="shared" ref="G202:J202" si="40">SUM(G201,G199,G197)</f>
+        <f t="shared" ref="G202:J202" si="45">SUM(G201,G199,G197)</f>
         <v>4068</v>
       </c>
       <c r="H202" s="107">
-        <f t="shared" si="40"/>
+        <f t="shared" si="45"/>
         <v>4398</v>
       </c>
       <c r="I202" s="107">
-        <f t="shared" si="40"/>
+        <f t="shared" si="45"/>
         <v>4819</v>
       </c>
       <c r="J202" s="107">
-        <f t="shared" si="40"/>
+        <f t="shared" si="45"/>
         <v>4992</v>
       </c>
       <c r="K202" s="105"/>
@@ -6997,19 +7326,19 @@
         <v>77700</v>
       </c>
       <c r="G207" s="28">
-        <f t="shared" ref="G207:J207" si="41">(G194+F194)/2</f>
+        <f t="shared" ref="G207:J207" si="46">(G194+F194)/2</f>
         <v>84000</v>
       </c>
       <c r="H207" s="28">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>91100</v>
       </c>
       <c r="I207" s="28">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>99100</v>
       </c>
       <c r="J207" s="28">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>107450</v>
       </c>
       <c r="K207" s="8"/>
@@ -7138,19 +7467,19 @@
         <v>48.435957154090985</v>
       </c>
       <c r="L213" s="164">
-        <f t="shared" ref="L213:O213" si="42">L26</f>
+        <f t="shared" ref="L213:O213" si="47">L26</f>
         <v>50.497236986532279</v>
       </c>
       <c r="M213" s="164">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>50.541197440064622</v>
       </c>
       <c r="N213" s="164">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>50.585196163442809</v>
       </c>
       <c r="O213" s="164">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>50.629233189982713</v>
       </c>
     </row>
@@ -7192,39 +7521,39 @@
         <v>782</v>
       </c>
       <c r="G216" s="28">
-        <f t="shared" ref="G216:O216" si="43">F218</f>
+        <f t="shared" ref="G216:O216" si="48">F218</f>
         <v>795</v>
       </c>
       <c r="H216" s="28">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>815</v>
       </c>
       <c r="I216" s="28">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>838</v>
       </c>
       <c r="J216" s="28">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>861</v>
       </c>
       <c r="K216" s="29">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>890</v>
       </c>
       <c r="L216" s="29">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>916</v>
       </c>
       <c r="M216" s="29">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>943</v>
       </c>
       <c r="N216" s="29">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>970</v>
       </c>
       <c r="O216" s="29">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>997</v>
       </c>
       <c r="P216" s="28"/>
@@ -7290,39 +7619,39 @@
         <v>795</v>
       </c>
       <c r="G218" s="30">
-        <f t="shared" ref="G218:O218" si="44">G217+G216</f>
+        <f t="shared" ref="G218:O218" si="49">G217+G216</f>
         <v>815</v>
       </c>
       <c r="H218" s="30">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>838</v>
       </c>
       <c r="I218" s="30">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>861</v>
       </c>
       <c r="J218" s="30">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>890</v>
       </c>
       <c r="K218" s="31">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>916</v>
       </c>
       <c r="L218" s="31">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>943</v>
       </c>
       <c r="M218" s="31">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>970</v>
       </c>
       <c r="N218" s="31">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>997</v>
       </c>
       <c r="O218" s="31">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>1024</v>
       </c>
       <c r="P218" s="28"/>
@@ -7346,39 +7675,39 @@
         <v>8.3120204603580571E-3</v>
       </c>
       <c r="G220" s="108">
-        <f t="shared" ref="G220:O220" si="45">G217/G216/2</f>
+        <f t="shared" ref="G220:O220" si="50">G217/G216/2</f>
         <v>1.2578616352201259E-2</v>
       </c>
       <c r="H220" s="108">
-        <f t="shared" si="45"/>
+        <f t="shared" si="50"/>
         <v>1.4110429447852761E-2</v>
       </c>
       <c r="I220" s="108">
-        <f t="shared" si="45"/>
+        <f t="shared" si="50"/>
         <v>1.3723150357995227E-2</v>
       </c>
       <c r="J220" s="108">
-        <f t="shared" si="45"/>
+        <f t="shared" si="50"/>
         <v>1.6840882694541232E-2</v>
       </c>
       <c r="K220" s="114">
-        <f t="shared" si="45"/>
+        <f t="shared" si="50"/>
         <v>1.4606741573033709E-2</v>
       </c>
       <c r="L220" s="114">
-        <f t="shared" si="45"/>
+        <f t="shared" si="50"/>
         <v>1.4737991266375546E-2</v>
       </c>
       <c r="M220" s="114">
-        <f t="shared" si="45"/>
+        <f t="shared" si="50"/>
         <v>1.4316012725344645E-2</v>
       </c>
       <c r="N220" s="114">
-        <f t="shared" si="45"/>
+        <f t="shared" si="50"/>
         <v>1.3917525773195877E-2</v>
       </c>
       <c r="O220" s="114">
-        <f t="shared" si="45"/>
+        <f t="shared" si="50"/>
         <v>1.354062186559679E-2</v>
       </c>
     </row>
@@ -7401,19 +7730,19 @@
         <v>6.7307692307692291E-2</v>
       </c>
       <c r="G222" s="108">
-        <f t="shared" ref="G222:J222" si="46">G207/F207-1</f>
+        <f t="shared" ref="G222:J222" si="51">G207/F207-1</f>
         <v>8.1081081081081141E-2</v>
       </c>
       <c r="H222" s="108">
-        <f t="shared" si="46"/>
+        <f t="shared" si="51"/>
         <v>8.4523809523809446E-2</v>
       </c>
       <c r="I222" s="108">
-        <f t="shared" si="46"/>
+        <f t="shared" si="51"/>
         <v>8.7815587266739881E-2</v>
       </c>
       <c r="J222" s="108">
-        <f t="shared" si="46"/>
+        <f t="shared" si="51"/>
         <v>8.425832492431895E-2</v>
       </c>
       <c r="K222" s="8"/>
@@ -7436,19 +7765,19 @@
         <v>5.8509341007755733E-2</v>
       </c>
       <c r="G223" s="158">
-        <f t="shared" ref="G223:J223" si="47">(1+G222)/(1+G220) -1</f>
+        <f t="shared" ref="G223:J223" si="52">(1+G222)/(1+G220) -1</f>
         <v>6.765150243411111E-2</v>
       </c>
       <c r="H223" s="158">
-        <f t="shared" si="47"/>
+        <f t="shared" si="52"/>
         <v>6.9433641575202376E-2</v>
       </c>
       <c r="I223" s="158">
-        <f t="shared" si="47"/>
+        <f t="shared" si="52"/>
         <v>7.3089419811098288E-2</v>
       </c>
       <c r="J223" s="158">
-        <f t="shared" si="47"/>
+        <f t="shared" si="52"/>
         <v>6.6300876938707676E-2</v>
       </c>
       <c r="K223" s="105"/>
@@ -7524,39 +7853,39 @@
         <v>5.8509341007755733E-2</v>
       </c>
       <c r="G226" s="108">
-        <f t="shared" ref="G226:O226" si="48">IF(G225=364,G223,(G223/371)*364)</f>
+        <f t="shared" ref="G226:O226" si="53">IF(G225=364,G223,(G223/371)*364)</f>
         <v>6.765150243411111E-2</v>
       </c>
       <c r="H226" s="108">
-        <f t="shared" si="48"/>
+        <f t="shared" si="53"/>
         <v>6.9433641575202376E-2</v>
       </c>
       <c r="I226" s="108">
-        <f t="shared" si="48"/>
+        <f t="shared" si="53"/>
         <v>7.1710374154285106E-2</v>
       </c>
       <c r="J226" s="108">
-        <f t="shared" si="48"/>
+        <f t="shared" si="53"/>
         <v>6.6300876938707676E-2</v>
       </c>
       <c r="K226" s="114">
-        <f t="shared" si="48"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="L226" s="114">
-        <f t="shared" si="48"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="M226" s="114">
-        <f t="shared" si="48"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="N226" s="114">
-        <f t="shared" si="48"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="O226" s="114">
-        <f t="shared" si="48"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
     </row>
@@ -7576,19 +7905,19 @@
         <v>6.8774098775576567E-2</v>
       </c>
       <c r="L227" s="161">
-        <f t="shared" ref="L227:O227" si="49">IF(L225=364,$J$227,($J$227*371)/364)</f>
+        <f t="shared" ref="L227:O227" si="54">IF(L225=364,$J$227,($J$227*371)/364)</f>
         <v>6.8774098775576567E-2</v>
       </c>
       <c r="M227" s="161">
-        <f t="shared" si="49"/>
+        <f t="shared" si="54"/>
         <v>6.8774098775576567E-2</v>
       </c>
       <c r="N227" s="161">
-        <f t="shared" si="49"/>
+        <f t="shared" si="54"/>
         <v>7.0096677598183804E-2</v>
       </c>
       <c r="O227" s="161">
-        <f t="shared" si="49"/>
+        <f t="shared" si="54"/>
         <v>6.8774098775576567E-2</v>
       </c>
     </row>
@@ -7611,19 +7940,19 @@
         <v>8.3380840348610277E-2</v>
       </c>
       <c r="L228" s="163">
-        <f t="shared" ref="L228:O228" si="50">L220+L227</f>
+        <f t="shared" ref="L228:O228" si="55">L220+L227</f>
         <v>8.3512090041952119E-2</v>
       </c>
       <c r="M228" s="163">
-        <f t="shared" si="50"/>
+        <f t="shared" si="55"/>
         <v>8.3090111500921215E-2</v>
       </c>
       <c r="N228" s="163">
-        <f t="shared" si="50"/>
+        <f t="shared" si="55"/>
         <v>8.4014203371379687E-2</v>
       </c>
       <c r="O228" s="163">
-        <f t="shared" si="50"/>
+        <f t="shared" si="55"/>
         <v>8.2314720641173358E-2</v>
       </c>
     </row>
@@ -7653,19 +7982,19 @@
         <v>120905.30178290491</v>
       </c>
       <c r="L230" s="29">
-        <f t="shared" ref="L230:O230" si="51">K230*(1+L228)</f>
+        <f t="shared" ref="L230:O230" si="56">K230*(1+L228)</f>
         <v>131002.35623194826</v>
       </c>
       <c r="M230" s="29">
-        <f t="shared" si="51"/>
+        <f t="shared" si="56"/>
         <v>141887.35661814426</v>
       </c>
       <c r="N230" s="29">
-        <f t="shared" si="51"/>
+        <f t="shared" si="56"/>
         <v>153807.90985288852</v>
       </c>
       <c r="O230" s="29">
-        <f t="shared" si="51"/>
+        <f t="shared" si="56"/>
         <v>166468.56498483181</v>
       </c>
     </row>
@@ -7684,19 +8013,19 @@
         <v>48.435957154090985</v>
       </c>
       <c r="L231" s="164">
-        <f t="shared" ref="L231:O231" si="52">L213</f>
+        <f t="shared" ref="L231:O231" si="57">L213</f>
         <v>50.497236986532279</v>
       </c>
       <c r="M231" s="164">
-        <f t="shared" si="52"/>
+        <f t="shared" si="57"/>
         <v>50.541197440064622</v>
       </c>
       <c r="N231" s="164">
-        <f t="shared" si="52"/>
+        <f t="shared" si="57"/>
         <v>50.585196163442809</v>
       </c>
       <c r="O231" s="164">
-        <f t="shared" si="52"/>
+        <f t="shared" si="57"/>
         <v>50.629233189982713</v>
       </c>
     </row>
@@ -7719,19 +8048,19 @@
         <v>5630.808417627888</v>
       </c>
       <c r="L232" s="168">
-        <f t="shared" ref="L232:O232" si="53">L231*(AVERAGE(K230:L230)/1000)</f>
+        <f t="shared" ref="L232:O232" si="58">L231*(AVERAGE(K230:L230)/1000)</f>
         <v>6360.3203527491833</v>
       </c>
       <c r="M232" s="168">
-        <f t="shared" si="53"/>
+        <f t="shared" si="58"/>
         <v>6896.0864282595321</v>
       </c>
       <c r="N232" s="168">
-        <f t="shared" si="53"/>
+        <f t="shared" si="58"/>
         <v>7478.9015295193431</v>
       </c>
       <c r="O232" s="168">
-        <f t="shared" si="53"/>
+        <f t="shared" si="58"/>
         <v>8107.6761649122873</v>
       </c>
     </row>
@@ -7758,19 +8087,19 @@
         <v>2798.6149845375976</v>
       </c>
       <c r="L234" s="175">
-        <f t="shared" ref="L234:O234" si="54">L232*$J$205</f>
+        <f t="shared" ref="L234:O234" si="59">L232*$J$205</f>
         <v>3161.1957867254223</v>
       </c>
       <c r="M234" s="175">
-        <f t="shared" si="54"/>
+        <f t="shared" si="59"/>
         <v>3427.4813457290124</v>
       </c>
       <c r="N234" s="175">
-        <f t="shared" si="54"/>
+        <f t="shared" si="59"/>
         <v>3717.1511328406177</v>
       </c>
       <c r="O234" s="175">
-        <f t="shared" si="54"/>
+        <f t="shared" si="59"/>
         <v>4029.6636507588128</v>
       </c>
     </row>
@@ -7786,19 +8115,19 @@
         <v>297.61498453759759</v>
       </c>
       <c r="L235" s="175">
-        <f t="shared" ref="L235:O235" si="55">L234-K234</f>
+        <f t="shared" ref="L235:O235" si="60">L234-K234</f>
         <v>362.5808021878247</v>
       </c>
       <c r="M235" s="175">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>266.28555900359015</v>
       </c>
       <c r="N235" s="175">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>289.66978711160527</v>
       </c>
       <c r="O235" s="175">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>312.51251791819504</v>
       </c>
     </row>
@@ -7821,19 +8150,19 @@
         <v>5333.1934330902905</v>
       </c>
       <c r="L236" s="201">
-        <f t="shared" ref="L236:O236" si="56">L232-L235</f>
+        <f t="shared" ref="L236:O236" si="61">L232-L235</f>
         <v>5997.7395505613586</v>
       </c>
       <c r="M236" s="201">
-        <f t="shared" si="56"/>
+        <f t="shared" si="61"/>
         <v>6629.8008692559415</v>
       </c>
       <c r="N236" s="201">
-        <f t="shared" si="56"/>
+        <f t="shared" si="61"/>
         <v>7189.2317424077373</v>
       </c>
       <c r="O236" s="201">
-        <f t="shared" si="56"/>
+        <f t="shared" si="61"/>
         <v>7795.1636469940922</v>
       </c>
     </row>
@@ -7892,39 +8221,39 @@
         <v>788.5</v>
       </c>
       <c r="G240" s="28">
-        <f t="shared" ref="G240:O240" si="57">(G216+G218)/2</f>
+        <f t="shared" ref="G240:O240" si="62">(G216+G218)/2</f>
         <v>805</v>
       </c>
       <c r="H240" s="28">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>826.5</v>
       </c>
       <c r="I240" s="28">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>849.5</v>
       </c>
       <c r="J240" s="28">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>875.5</v>
       </c>
       <c r="K240" s="29">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>903</v>
       </c>
       <c r="L240" s="29">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>929.5</v>
       </c>
       <c r="M240" s="29">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>956.5</v>
       </c>
       <c r="N240" s="29">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>983.5</v>
       </c>
       <c r="O240" s="29">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>1010.5</v>
       </c>
     </row>
@@ -7941,43 +8270,43 @@
         <v>113.48399999999999</v>
       </c>
       <c r="F241" s="30">
-        <f t="shared" ref="F241:O241" si="58">(F240*$F$239)/1000</f>
+        <f t="shared" ref="F241:O241" si="63">(F240*$F$239)/1000</f>
         <v>115.90949999999999</v>
       </c>
       <c r="G241" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>118.33499999999999</v>
       </c>
       <c r="H241" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>121.49550000000001</v>
       </c>
       <c r="I241" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>124.87649999999999</v>
       </c>
       <c r="J241" s="30">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>128.6985</v>
       </c>
       <c r="K241" s="31">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>132.74100000000001</v>
       </c>
       <c r="L241" s="31">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>136.63650000000001</v>
       </c>
       <c r="M241" s="31">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>140.60550000000001</v>
       </c>
       <c r="N241" s="31">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>144.5745</v>
       </c>
       <c r="O241" s="31">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>148.54349999999999</v>
       </c>
     </row>
@@ -8026,19 +8355,19 @@
         <v>1180</v>
       </c>
       <c r="G244" s="28">
-        <f t="shared" ref="G244:J244" si="59">F248</f>
+        <f t="shared" ref="G244:J244" si="64">F248</f>
         <v>1393</v>
       </c>
       <c r="H244" s="28">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>1671</v>
       </c>
       <c r="I244" s="28">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>1911</v>
       </c>
       <c r="J244" s="28">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>2150</v>
       </c>
       <c r="K244" s="29"/>
@@ -8089,23 +8418,23 @@
         <v>0</v>
       </c>
       <c r="F246" s="30">
-        <f t="shared" ref="F246:J246" si="60">F244+F245</f>
+        <f t="shared" ref="F246:J246" si="65">F244+F245</f>
         <v>2887</v>
       </c>
       <c r="G246" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>3440</v>
       </c>
       <c r="H246" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>3978</v>
       </c>
       <c r="I246" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>4487</v>
       </c>
       <c r="J246" s="30">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>4954</v>
       </c>
       <c r="K246" s="31"/>
@@ -8176,23 +8505,23 @@
         <v>-1180</v>
       </c>
       <c r="F249" s="30">
-        <f t="shared" ref="F249:J249" si="61">F246-F248</f>
+        <f t="shared" ref="F249:J249" si="66">F246-F248</f>
         <v>1494</v>
       </c>
       <c r="G249" s="30">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>1769</v>
       </c>
       <c r="H249" s="30">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>2067</v>
       </c>
       <c r="I249" s="30">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>2337</v>
       </c>
       <c r="J249" s="30">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>2519</v>
       </c>
       <c r="K249" s="31"/>
@@ -8233,15 +8562,15 @@
         <v>278</v>
       </c>
       <c r="H251" s="28">
-        <f t="shared" ref="H251:J251" si="62">H248-G248</f>
+        <f t="shared" ref="H251:J251" si="67">H248-G248</f>
         <v>240</v>
       </c>
       <c r="I251" s="28">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>239</v>
       </c>
       <c r="J251" s="28">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>285</v>
       </c>
       <c r="K251" s="29"/>
@@ -8312,23 +8641,23 @@
         <v>149474</v>
       </c>
       <c r="F254" s="30">
-        <f t="shared" ref="F254:J254" si="63">SUM(F253,F251)</f>
+        <f t="shared" ref="F254:J254" si="68">SUM(F253,F251)</f>
         <v>163433</v>
       </c>
       <c r="G254" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>192330</v>
       </c>
       <c r="H254" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>222970</v>
       </c>
       <c r="I254" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>237949</v>
       </c>
       <c r="J254" s="30">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>249910</v>
       </c>
       <c r="K254" s="31"/>
@@ -8356,23 +8685,23 @@
         <v>1317.1372175813331</v>
       </c>
       <c r="F256" s="28">
-        <f t="shared" ref="F256:J256" si="64">F254/F241</f>
+        <f t="shared" ref="F256:J256" si="69">F254/F241</f>
         <v>1410.0052195894211</v>
       </c>
       <c r="G256" s="28">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>1625.3010520978578</v>
       </c>
       <c r="H256" s="28">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>1835.2120037367638</v>
       </c>
       <c r="I256" s="28">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>1905.4746089136067</v>
       </c>
       <c r="J256" s="28">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>1941.82527379884</v>
       </c>
       <c r="K256" s="8"/>
@@ -8400,19 +8729,19 @@
         <v>7.0507461765162205E-2</v>
       </c>
       <c r="G258" s="108">
-        <f t="shared" ref="G258:J258" si="65">(G256/F256)-1</f>
+        <f t="shared" ref="G258:J258" si="70">(G256/F256)-1</f>
         <v>0.15269151455420049</v>
       </c>
       <c r="H258" s="108">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>0.1291520431663804</v>
       </c>
       <c r="I258" s="108">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>3.8285824762358756E-2</v>
       </c>
       <c r="J258" s="108">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>1.9076961044344865E-2</v>
       </c>
       <c r="K258" s="186">
@@ -8448,39 +8777,39 @@
         <v>2.1373056994818729E-2</v>
       </c>
       <c r="G259" s="108">
-        <f t="shared" ref="G259:O259" si="66">(G241/F241)-1</f>
+        <f t="shared" ref="G259:O259" si="71">(G241/F241)-1</f>
         <v>2.0925808497146425E-2</v>
       </c>
       <c r="H259" s="108">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>2.6708074534161685E-2</v>
       </c>
       <c r="I259" s="108">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>2.7828191167573957E-2</v>
       </c>
       <c r="J259" s="108">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>3.0606238964096644E-2</v>
       </c>
       <c r="K259" s="114">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>3.1410622501427898E-2</v>
       </c>
       <c r="L259" s="114">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>2.9346622369878173E-2</v>
       </c>
       <c r="M259" s="114">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>2.9047875201721363E-2</v>
       </c>
       <c r="N259" s="114">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>2.8227914270778864E-2</v>
       </c>
       <c r="O259" s="114">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>2.7452974072191161E-2</v>
       </c>
     </row>
@@ -8503,39 +8832,39 @@
         <v>9.3387478758847786E-2</v>
       </c>
       <c r="G261" s="108">
-        <f t="shared" ref="G261:O261" si="67">(1+G258)*(1+G259)-1</f>
+        <f t="shared" ref="G261:O261" si="72">(1+G258)*(1+G259)-1</f>
         <v>0.17681251644404727</v>
       </c>
       <c r="H261" s="108">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>0.15930952009566912</v>
       </c>
       <c r="I261" s="108">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>6.7179441180427846E-2</v>
       </c>
       <c r="J261" s="108">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>5.0267074036873582E-2</v>
       </c>
       <c r="K261" s="114">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>7.5372866383931258E-2</v>
       </c>
       <c r="L261" s="114">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>7.6308931383554546E-2</v>
       </c>
       <c r="M261" s="114">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>7.908369797471404E-2</v>
       </c>
       <c r="N261" s="114">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>8.1308551485251845E-2</v>
       </c>
       <c r="O261" s="114">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>8.3575965148744435E-2</v>
       </c>
     </row>
@@ -8597,19 +8926,19 @@
         <v>1707</v>
       </c>
       <c r="G265" s="104">
-        <f t="shared" ref="G265:J265" si="68">G245</f>
+        <f t="shared" ref="G265:J265" si="73">G245</f>
         <v>2047</v>
       </c>
       <c r="H265" s="104">
-        <f t="shared" si="68"/>
+        <f t="shared" si="73"/>
         <v>2307</v>
       </c>
       <c r="I265" s="104">
-        <f t="shared" si="68"/>
+        <f t="shared" si="73"/>
         <v>2576</v>
       </c>
       <c r="J265" s="104">
-        <f t="shared" si="68"/>
+        <f t="shared" si="73"/>
         <v>2804</v>
       </c>
       <c r="K265" s="8"/>
@@ -8630,19 +8959,19 @@
         <v>1.0444647041907082E-2</v>
       </c>
       <c r="G266" s="108">
-        <f t="shared" ref="G266:J266" si="69">G265/G254</f>
+        <f t="shared" ref="G266:J266" si="74">G265/G254</f>
         <v>1.0643165392814433E-2</v>
       </c>
       <c r="H266" s="108">
-        <f t="shared" si="69"/>
+        <f t="shared" si="74"/>
         <v>1.034668341032426E-2</v>
       </c>
       <c r="I266" s="108">
-        <f t="shared" si="69"/>
+        <f t="shared" si="74"/>
         <v>1.0825849236601121E-2</v>
       </c>
       <c r="J266" s="108">
-        <f t="shared" si="69"/>
+        <f t="shared" si="74"/>
         <v>1.1220039214117083E-2</v>
       </c>
       <c r="K266" s="185">
@@ -8686,19 +9015,19 @@
         <v>0.87521968365553604</v>
       </c>
       <c r="G268" s="108">
-        <f t="shared" ref="G268:J268" si="70">G249/G245</f>
+        <f t="shared" ref="G268:J268" si="75">G249/G245</f>
         <v>0.86419149975574006</v>
       </c>
       <c r="H268" s="108">
-        <f t="shared" si="70"/>
+        <f t="shared" si="75"/>
         <v>0.89596879063719115</v>
       </c>
       <c r="I268" s="108">
-        <f t="shared" si="70"/>
+        <f t="shared" si="75"/>
         <v>0.90722049689440998</v>
       </c>
       <c r="J268" s="108">
-        <f t="shared" si="70"/>
+        <f t="shared" si="75"/>
         <v>0.89835948644793151</v>
       </c>
       <c r="K268" s="8"/>
@@ -8760,19 +9089,19 @@
         <v>2435</v>
       </c>
       <c r="L272" s="175">
-        <f t="shared" ref="L272:O272" si="71">K276</f>
+        <f t="shared" ref="L272:O272" si="76">K276</f>
         <v>2778.1493779941638</v>
       </c>
       <c r="M272" s="175">
-        <f t="shared" si="71"/>
+        <f t="shared" si="76"/>
         <v>3153.9523052301415</v>
       </c>
       <c r="N272" s="175">
-        <f t="shared" si="71"/>
+        <f t="shared" si="76"/>
         <v>3566.4548327032235</v>
       </c>
       <c r="O272" s="175">
-        <f t="shared" si="71"/>
+        <f t="shared" si="76"/>
         <v>4020.0445687305178</v>
       </c>
     </row>
@@ -8792,19 +9121,19 @@
         <v>3069.0948039481455</v>
       </c>
       <c r="L273" s="167">
-        <f t="shared" ref="L273:O273" si="72">L263*L266</f>
+        <f t="shared" ref="L273:O273" si="77">L263*L266</f>
         <v>3361.1449859835047</v>
       </c>
       <c r="M273" s="167">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>3689.3826562746854</v>
       </c>
       <c r="N273" s="167">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>4056.8626704293683</v>
       </c>
       <c r="O273" s="167">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>4469.0620540084155</v>
       </c>
     </row>
@@ -8826,23 +9155,23 @@
         <v>4954</v>
       </c>
       <c r="K274" s="168">
-        <f t="shared" ref="K274:O274" si="73">SUM(K272:K273)</f>
+        <f t="shared" ref="K274:O274" si="78">SUM(K272:K273)</f>
         <v>5504.0948039481455</v>
       </c>
       <c r="L274" s="168">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>6139.2943639776686</v>
       </c>
       <c r="M274" s="168">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>6843.3349615048264</v>
       </c>
       <c r="N274" s="168">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>7623.3175031325918</v>
       </c>
       <c r="O274" s="168">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>8489.1066227389329</v>
       </c>
     </row>
@@ -8862,19 +9191,19 @@
         <v>2725.9454259539816</v>
       </c>
       <c r="L275" s="167">
-        <f t="shared" ref="L275:O275" si="74">L273*$J$269</f>
+        <f t="shared" ref="L275:O275" si="79">L273*$J$269</f>
         <v>2985.3420587475271</v>
       </c>
       <c r="M275" s="167">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>3276.880128801603</v>
       </c>
       <c r="N275" s="167">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>3603.272934402074</v>
       </c>
       <c r="O275" s="167">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>3969.3851257892188</v>
       </c>
     </row>
@@ -8896,23 +9225,23 @@
         <v>2435</v>
       </c>
       <c r="K276" s="168">
-        <f t="shared" ref="K276:O276" si="75">K274-K275</f>
+        <f t="shared" ref="K276:O276" si="80">K274-K275</f>
         <v>2778.1493779941638</v>
       </c>
       <c r="L276" s="168">
-        <f t="shared" si="75"/>
+        <f t="shared" si="80"/>
         <v>3153.9523052301415</v>
       </c>
       <c r="M276" s="168">
-        <f t="shared" si="75"/>
+        <f t="shared" si="80"/>
         <v>3566.4548327032235</v>
       </c>
       <c r="N276" s="168">
-        <f t="shared" si="75"/>
+        <f t="shared" si="80"/>
         <v>4020.0445687305178</v>
       </c>
       <c r="O276" s="168">
-        <f t="shared" si="75"/>
+        <f t="shared" si="80"/>
         <v>4519.7214969497145</v>
       </c>
     </row>
@@ -8935,19 +9264,19 @@
         <v>343.14937799416384</v>
       </c>
       <c r="L278" s="175">
-        <f t="shared" ref="L278:O278" si="76">L276-K276</f>
+        <f t="shared" ref="L278:O278" si="81">L276-K276</f>
         <v>375.80292723597768</v>
       </c>
       <c r="M278" s="175">
-        <f t="shared" si="76"/>
+        <f t="shared" si="81"/>
         <v>412.50252747308195</v>
       </c>
       <c r="N278" s="175">
-        <f t="shared" si="76"/>
+        <f t="shared" si="81"/>
         <v>453.58973602729429</v>
       </c>
       <c r="O278" s="175">
-        <f t="shared" si="76"/>
+        <f t="shared" si="81"/>
         <v>499.67692821919672</v>
       </c>
     </row>
@@ -8970,19 +9299,19 @@
         <v>268403.2836600141</v>
       </c>
       <c r="L279" s="101">
-        <f t="shared" ref="L279:O279" si="77">L263-L278</f>
+        <f t="shared" ref="L279:O279" si="82">L263-L278</f>
         <v>288878.38322904473</v>
       </c>
       <c r="M279" s="101">
-        <f t="shared" si="77"/>
+        <f t="shared" si="82"/>
         <v>311716.97432471259</v>
       </c>
       <c r="N279" s="101">
-        <f t="shared" si="77"/>
+        <f t="shared" si="82"/>
         <v>337054.68275485904</v>
       </c>
       <c r="O279" s="101">
-        <f t="shared" si="77"/>
+        <f t="shared" si="82"/>
         <v>365216.17518177838</v>
       </c>
     </row>
@@ -9017,23 +9346,23 @@
       <c r="D284" s="2"/>
       <c r="E284" s="4"/>
       <c r="F284" s="4">
-        <f t="shared" ref="F284:J284" si="78">G284-1</f>
+        <f t="shared" ref="F284:J284" si="83">G284-1</f>
         <v>2020</v>
       </c>
       <c r="G284" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="83"/>
         <v>2021</v>
       </c>
       <c r="H284" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="83"/>
         <v>2022</v>
       </c>
       <c r="I284" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="83"/>
         <v>2023</v>
       </c>
       <c r="J284" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="83"/>
         <v>2024</v>
       </c>
       <c r="K284" s="7">
@@ -9152,19 +9481,19 @@
         <v>0.11200220561205732</v>
       </c>
       <c r="G287" s="158">
-        <f t="shared" ref="G287:J287" si="79">1-(G286/G285)</f>
+        <f t="shared" ref="G287:J287" si="84">1-(G286/G285)</f>
         <v>0.11126153333472188</v>
       </c>
       <c r="H287" s="158">
-        <f t="shared" si="79"/>
+        <f t="shared" si="84"/>
         <v>0.10482647151259372</v>
       </c>
       <c r="I287" s="158">
-        <f t="shared" si="79"/>
+        <f t="shared" si="84"/>
         <v>0.10569180934752431</v>
       </c>
       <c r="J287" s="158">
-        <f t="shared" si="79"/>
+        <f t="shared" si="84"/>
         <v>0.10923184777165751</v>
       </c>
       <c r="K287" s="105"/>
@@ -9189,19 +9518,19 @@
         <v>0.10860277351571095</v>
       </c>
       <c r="L288" s="161">
-        <f t="shared" ref="L288:O288" si="80">L40</f>
+        <f t="shared" ref="L288:O288" si="85">L40</f>
         <v>0.10860277351571095</v>
       </c>
       <c r="M288" s="161">
-        <f t="shared" si="80"/>
+        <f t="shared" si="85"/>
         <v>0.10860277351571095</v>
       </c>
       <c r="N288" s="161">
-        <f t="shared" si="80"/>
+        <f t="shared" si="85"/>
         <v>0.10860277351571095</v>
       </c>
       <c r="O288" s="161">
-        <f t="shared" si="80"/>
+        <f t="shared" si="85"/>
         <v>0.10860277351571095</v>
       </c>
     </row>
@@ -9295,19 +9624,19 @@
         <v>0.10039823551035412</v>
       </c>
       <c r="G292" s="108">
-        <f t="shared" ref="G292:J292" si="81">G291/G285</f>
+        <f t="shared" ref="G292:J292" si="86">G291/G285</f>
         <v>9.6520733967883701E-2</v>
       </c>
       <c r="H292" s="108">
-        <f t="shared" si="81"/>
+        <f t="shared" si="86"/>
         <v>8.8802586090782565E-2</v>
       </c>
       <c r="I292" s="108">
-        <f t="shared" si="81"/>
+        <f t="shared" si="86"/>
         <v>9.0824954776828906E-2</v>
       </c>
       <c r="J292" s="108">
-        <f t="shared" si="81"/>
+        <f t="shared" si="86"/>
         <v>9.1377065598397603E-2</v>
       </c>
       <c r="K292" s="8"/>
@@ -9328,23 +9657,23 @@
         <v>9.1881335108473183E-2</v>
       </c>
       <c r="K293" s="161">
-        <f t="shared" ref="K293:O293" si="82">K42</f>
+        <f t="shared" ref="K293:O293" si="87">K42</f>
         <v>9.0297304168993064E-2</v>
       </c>
       <c r="L293" s="161">
-        <f t="shared" si="82"/>
+        <f t="shared" si="87"/>
         <v>8.8713273229512946E-2</v>
       </c>
       <c r="M293" s="161">
-        <f t="shared" si="82"/>
+        <f t="shared" si="87"/>
         <v>8.7129242290032827E-2</v>
       </c>
       <c r="N293" s="161">
-        <f t="shared" si="82"/>
+        <f t="shared" si="87"/>
         <v>8.5545211350552708E-2</v>
       </c>
       <c r="O293" s="161">
-        <f t="shared" si="82"/>
+        <f t="shared" si="87"/>
         <v>8.3961180411072589E-2</v>
       </c>
     </row>
@@ -9450,19 +9779,19 @@
         <v>24236.092944604818</v>
       </c>
       <c r="L299" s="166">
-        <f t="shared" ref="L299:O299" si="83">L293*L285</f>
+        <f t="shared" ref="L299:O299" si="88">L293*L285</f>
         <v>25627.346941498196</v>
       </c>
       <c r="M299" s="166">
-        <f t="shared" si="83"/>
+        <f t="shared" si="88"/>
         <v>27159.663781853826</v>
       </c>
       <c r="N299" s="166">
-        <f t="shared" si="83"/>
+        <f t="shared" si="88"/>
         <v>28833.414072957909</v>
       </c>
       <c r="O299" s="166">
-        <f t="shared" si="83"/>
+        <f t="shared" si="88"/>
         <v>30663.981173479187</v>
       </c>
     </row>
@@ -9518,19 +9847,19 @@
         <v>0.21999145664246048</v>
       </c>
       <c r="G302" s="108">
-        <f t="shared" ref="G302:J302" si="84">G301/G291</f>
+        <f t="shared" ref="G302:J302" si="89">G301/G291</f>
         <v>0.22063980147812484</v>
       </c>
       <c r="H302" s="108">
-        <f t="shared" si="84"/>
+        <f t="shared" si="89"/>
         <v>0.22149754790434298</v>
       </c>
       <c r="I302" s="108">
-        <f t="shared" si="84"/>
+        <f t="shared" si="89"/>
         <v>0.19814729041222789</v>
       </c>
       <c r="J302" s="108">
-        <f t="shared" si="84"/>
+        <f t="shared" si="89"/>
         <v>0.21017097764138537</v>
       </c>
       <c r="K302" s="8"/>
@@ -9559,19 +9888,19 @@
         <v>0.21408941481570834</v>
       </c>
       <c r="L303" s="161">
-        <f t="shared" ref="L303:O303" si="85">$J$303</f>
+        <f t="shared" ref="L303:O303" si="90">$J$303</f>
         <v>0.21408941481570834</v>
       </c>
       <c r="M303" s="161">
-        <f t="shared" si="85"/>
+        <f t="shared" si="90"/>
         <v>0.21408941481570834</v>
       </c>
       <c r="N303" s="161">
-        <f t="shared" si="85"/>
+        <f t="shared" si="90"/>
         <v>0.21408941481570834</v>
       </c>
       <c r="O303" s="161">
-        <f t="shared" si="85"/>
+        <f t="shared" si="90"/>
         <v>0.21408941481570834</v>
       </c>
     </row>
@@ -9587,19 +9916,19 @@
         <v>5188.6909559295627</v>
       </c>
       <c r="L304" s="167">
-        <f t="shared" ref="L304:O304" si="86">L303*L299</f>
+        <f t="shared" ref="L304:O304" si="91">L303*L299</f>
         <v>5486.5437099844812</v>
       </c>
       <c r="M304" s="167">
-        <f t="shared" si="86"/>
+        <f t="shared" si="91"/>
         <v>5814.5965256484733</v>
       </c>
       <c r="N304" s="167">
-        <f t="shared" si="86"/>
+        <f t="shared" si="91"/>
         <v>6172.9287460185678</v>
       </c>
       <c r="O304" s="167">
-        <f t="shared" si="86"/>
+        <f t="shared" si="91"/>
         <v>6564.833785350057</v>
       </c>
     </row>
@@ -9634,23 +9963,23 @@
       <c r="D309" s="2"/>
       <c r="E309" s="4"/>
       <c r="F309" s="4">
-        <f t="shared" ref="F309:J309" si="87">G309-1</f>
+        <f t="shared" ref="F309:J309" si="92">G309-1</f>
         <v>2020</v>
       </c>
       <c r="G309" s="4">
-        <f t="shared" si="87"/>
+        <f t="shared" si="92"/>
         <v>2021</v>
       </c>
       <c r="H309" s="4">
-        <f t="shared" si="87"/>
+        <f t="shared" si="92"/>
         <v>2022</v>
       </c>
       <c r="I309" s="4">
-        <f t="shared" si="87"/>
+        <f t="shared" si="92"/>
         <v>2023</v>
       </c>
       <c r="J309" s="4">
-        <f t="shared" si="87"/>
+        <f t="shared" si="92"/>
         <v>2024</v>
       </c>
       <c r="K309" s="7">
@@ -9728,19 +10057,19 @@
         <v>7.5225973600457019E-2</v>
       </c>
       <c r="L312" s="114">
-        <f t="shared" ref="L312:O312" si="88">(L311/K311)-1</f>
+        <f t="shared" ref="L312:O312" si="93">(L311/K311)-1</f>
         <v>7.6284832621371423E-2</v>
       </c>
       <c r="M312" s="114">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>7.9059536543998554E-2</v>
       </c>
       <c r="N312" s="114">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>8.1284339696408026E-2</v>
       </c>
       <c r="O312" s="114">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>8.3551702046523069E-2</v>
       </c>
     </row>
@@ -9788,19 +10117,19 @@
         <v>7.59853148247982E-2</v>
       </c>
       <c r="L314" s="114">
-        <f t="shared" ref="L314:O314" si="89">(L313/K313)-1</f>
+        <f t="shared" ref="L314:O314" si="94">(L313/K313)-1</f>
         <v>7.6284832621371201E-2</v>
       </c>
       <c r="M314" s="114">
-        <f t="shared" si="89"/>
+        <f t="shared" si="94"/>
         <v>7.9059536543998332E-2</v>
       </c>
       <c r="N314" s="114">
-        <f t="shared" si="89"/>
+        <f t="shared" si="94"/>
         <v>8.1284339696408026E-2</v>
       </c>
       <c r="O314" s="114">
-        <f t="shared" si="89"/>
+        <f t="shared" si="94"/>
         <v>8.3551702046523291E-2</v>
       </c>
     </row>
@@ -9834,19 +10163,19 @@
         <v>2925.6898741668438</v>
       </c>
       <c r="L317" s="29">
-        <f t="shared" ref="L317:O317" si="90">K317*(1+L312)</f>
+        <f t="shared" ref="L317:O317" si="95">K317*(1+L312)</f>
         <v>3148.8756365197028</v>
       </c>
       <c r="M317" s="29">
-        <f t="shared" si="90"/>
+        <f t="shared" si="95"/>
         <v>3397.8242849776389</v>
       </c>
       <c r="N317" s="29">
-        <f t="shared" si="90"/>
+        <f t="shared" si="95"/>
         <v>3674.0141883864658</v>
       </c>
       <c r="O317" s="29">
-        <f t="shared" si="90"/>
+        <f t="shared" si="95"/>
         <v>3980.9843271692303</v>
       </c>
     </row>
@@ -9863,19 +10192,19 @@
         <v>20063.898165538012</v>
       </c>
       <c r="L318" s="29">
-        <f t="shared" ref="L318:O318" si="91">K318*(1+L314)</f>
+        <f t="shared" ref="L318:O318" si="96">K318*(1+L314)</f>
         <v>21594.469278828317</v>
       </c>
       <c r="M318" s="29">
-        <f t="shared" si="91"/>
+        <f t="shared" si="96"/>
         <v>23301.718011926096</v>
       </c>
       <c r="N318" s="29">
-        <f t="shared" si="91"/>
+        <f t="shared" si="96"/>
         <v>25195.782774317406</v>
       </c>
       <c r="O318" s="29">
-        <f t="shared" si="91"/>
+        <f t="shared" si="96"/>
         <v>27300.933309506097</v>
       </c>
     </row>
@@ -9892,19 +10221,19 @@
         <v>1864.4418382231925</v>
       </c>
       <c r="L319" s="29">
-        <f t="shared" ref="L319:O319" si="92">K319*(1+L312)</f>
+        <f t="shared" ref="L319:O319" si="97">K319*(1+L312)</f>
         <v>2006.6704717843309</v>
       </c>
       <c r="M319" s="29">
-        <f t="shared" si="92"/>
+        <f t="shared" si="97"/>
         <v>2165.3169092801268</v>
       </c>
       <c r="N319" s="29">
-        <f t="shared" si="92"/>
+        <f t="shared" si="97"/>
         <v>2341.3232644844288</v>
       </c>
       <c r="O319" s="29">
-        <f t="shared" si="92"/>
+        <f t="shared" si="97"/>
         <v>2536.9448082732247</v>
       </c>
     </row>
@@ -9928,19 +10257,19 @@
         <v>20896.710799212407</v>
       </c>
       <c r="L321" s="29">
-        <f t="shared" ref="L321:O321" si="93">K321*(1+L314)</f>
+        <f t="shared" ref="L321:O321" si="98">K321*(1+L314)</f>
         <v>22490.812884867526</v>
       </c>
       <c r="M321" s="29">
-        <f t="shared" si="93"/>
+        <f t="shared" si="98"/>
         <v>24268.926128042938</v>
       </c>
       <c r="N321" s="29">
-        <f t="shared" si="93"/>
+        <f t="shared" si="98"/>
         <v>26241.609763501812</v>
       </c>
       <c r="O321" s="29">
-        <f t="shared" si="93"/>
+        <f t="shared" si="98"/>
         <v>28434.140923683051</v>
       </c>
     </row>
@@ -10044,19 +10373,19 @@
         <v>6677.1532960588384</v>
       </c>
       <c r="L325" s="29">
-        <f t="shared" ref="L325:O325" si="94">K325*(1+L312)</f>
+        <f t="shared" ref="L325:O325" si="99">K325*(1+L312)</f>
         <v>7186.5188176359252</v>
       </c>
       <c r="M325" s="29">
-        <f t="shared" si="94"/>
+        <f t="shared" si="99"/>
         <v>7754.6816647229462</v>
       </c>
       <c r="N325" s="29">
-        <f t="shared" si="94"/>
+        <f t="shared" si="99"/>
         <v>8385.0158433957931</v>
       </c>
       <c r="O325" s="29">
-        <f t="shared" si="94"/>
+        <f t="shared" si="99"/>
         <v>9085.5981887985745</v>
       </c>
     </row>
@@ -10076,19 +10405,19 @@
         <v>-1416.8981655380121</v>
       </c>
       <c r="L327" s="29">
-        <f t="shared" ref="L327:O327" si="95">K318-L318</f>
+        <f t="shared" ref="L327:O327" si="100">K318-L318</f>
         <v>-1530.5711132903052</v>
       </c>
       <c r="M327" s="29">
-        <f t="shared" si="95"/>
+        <f t="shared" si="100"/>
         <v>-1707.2487330977783</v>
       </c>
       <c r="N327" s="29">
-        <f t="shared" si="95"/>
+        <f t="shared" si="100"/>
         <v>-1894.0647623913101</v>
       </c>
       <c r="O327" s="29">
-        <f t="shared" si="95"/>
+        <f t="shared" si="100"/>
         <v>-2105.1505351886917</v>
       </c>
     </row>
@@ -10101,19 +10430,19 @@
         <v>1475.7107992124074</v>
       </c>
       <c r="L328" s="29">
-        <f t="shared" ref="L328:O328" si="96">L321-K321</f>
+        <f t="shared" ref="L328:O328" si="101">L321-K321</f>
         <v>1594.1020856551186</v>
       </c>
       <c r="M328" s="29">
-        <f t="shared" si="96"/>
+        <f t="shared" si="101"/>
         <v>1778.1132431754122</v>
       </c>
       <c r="N328" s="29">
-        <f t="shared" si="96"/>
+        <f t="shared" si="101"/>
         <v>1972.6836354588741</v>
       </c>
       <c r="O328" s="29">
-        <f t="shared" si="96"/>
+        <f t="shared" si="101"/>
         <v>2192.5311601812391</v>
       </c>
     </row>
@@ -10133,19 +10462,19 @@
         <v>-204.68987416684377</v>
       </c>
       <c r="L330" s="29">
-        <f t="shared" ref="L330:O330" si="97">K317-L317</f>
+        <f t="shared" ref="L330:O330" si="102">K317-L317</f>
         <v>-223.185762352859</v>
       </c>
       <c r="M330" s="29">
-        <f t="shared" si="97"/>
+        <f t="shared" si="102"/>
         <v>-248.94864845793609</v>
       </c>
       <c r="N330" s="29">
-        <f t="shared" si="97"/>
+        <f t="shared" si="102"/>
         <v>-276.18990340882692</v>
       </c>
       <c r="O330" s="29">
-        <f t="shared" si="97"/>
+        <f t="shared" si="102"/>
         <v>-306.97013878276448</v>
       </c>
     </row>
@@ -10158,19 +10487,19 @@
         <v>-130.44183822319246</v>
       </c>
       <c r="L331" s="29">
-        <f t="shared" ref="L331:O331" si="98">K319-L319</f>
+        <f t="shared" ref="L331:O331" si="103">K319-L319</f>
         <v>-142.22863356113839</v>
       </c>
       <c r="M331" s="29">
-        <f t="shared" si="98"/>
+        <f t="shared" si="103"/>
         <v>-158.64643749579591</v>
       </c>
       <c r="N331" s="29">
-        <f t="shared" si="98"/>
+        <f t="shared" si="103"/>
         <v>-176.00635520430205</v>
       </c>
       <c r="O331" s="29">
-        <f t="shared" si="98"/>
+        <f t="shared" si="103"/>
         <v>-195.62154378879586</v>
       </c>
     </row>
@@ -10191,19 +10520,19 @@
         <v>-335.13171239003623</v>
       </c>
       <c r="L332" s="31">
-        <f t="shared" ref="L332:O332" si="99">SUM(L330:L331)</f>
+        <f t="shared" ref="L332:O332" si="104">SUM(L330:L331)</f>
         <v>-365.4143959139974</v>
       </c>
       <c r="M332" s="31">
-        <f t="shared" si="99"/>
+        <f t="shared" si="104"/>
         <v>-407.595085953732</v>
       </c>
       <c r="N332" s="31">
-        <f t="shared" si="99"/>
+        <f t="shared" si="104"/>
         <v>-452.19625861312898</v>
       </c>
       <c r="O332" s="31">
-        <f t="shared" si="99"/>
+        <f t="shared" si="104"/>
         <v>-502.59168257156034</v>
       </c>
     </row>
@@ -10223,19 +10552,19 @@
         <v>394.69095592956273</v>
       </c>
       <c r="L334" s="29">
-        <f t="shared" ref="L334:O334" si="100">L322-K322</f>
+        <f t="shared" ref="L334:O334" si="105">L322-K322</f>
         <v>297.85275405491848</v>
       </c>
       <c r="M334" s="29">
-        <f t="shared" si="100"/>
+        <f t="shared" si="105"/>
         <v>328.05281566399208</v>
       </c>
       <c r="N334" s="29">
-        <f t="shared" si="100"/>
+        <f t="shared" si="105"/>
         <v>358.33222037009455</v>
       </c>
       <c r="O334" s="29">
-        <f t="shared" si="100"/>
+        <f t="shared" si="105"/>
         <v>391.90503933148921</v>
       </c>
     </row>
@@ -10248,19 +10577,19 @@
         <v>343.14937799416384</v>
       </c>
       <c r="L335" s="29">
-        <f t="shared" ref="L335:O335" si="101">L323-K323</f>
+        <f t="shared" ref="L335:O335" si="106">L323-K323</f>
         <v>375.80292723597768</v>
       </c>
       <c r="M335" s="29">
-        <f t="shared" si="101"/>
+        <f t="shared" si="106"/>
         <v>412.50252747308195</v>
       </c>
       <c r="N335" s="29">
-        <f t="shared" si="101"/>
+        <f t="shared" si="106"/>
         <v>453.58973602729429</v>
       </c>
       <c r="O335" s="29">
-        <f t="shared" si="101"/>
+        <f t="shared" si="106"/>
         <v>499.67692821919672</v>
       </c>
     </row>
@@ -10273,19 +10602,19 @@
         <v>297.61498453759759</v>
       </c>
       <c r="L336" s="29">
-        <f t="shared" ref="L336:O336" si="102">L324-K324</f>
+        <f t="shared" ref="L336:O336" si="107">L324-K324</f>
         <v>362.5808021878247</v>
       </c>
       <c r="M336" s="29">
-        <f t="shared" si="102"/>
+        <f t="shared" si="107"/>
         <v>266.28555900359015</v>
       </c>
       <c r="N336" s="29">
-        <f t="shared" si="102"/>
+        <f t="shared" si="107"/>
         <v>289.66978711160527</v>
       </c>
       <c r="O336" s="29">
-        <f t="shared" si="102"/>
+        <f t="shared" si="107"/>
         <v>312.51251791819504</v>
       </c>
     </row>
@@ -10298,23 +10627,24 @@
         <v>467.15329605883835</v>
       </c>
       <c r="L337" s="29">
-        <f t="shared" ref="L337:O337" si="103">L325-K325</f>
+        <f t="shared" ref="L337:O337" si="108">L325-K325</f>
         <v>509.36552157708684</v>
       </c>
       <c r="M337" s="29">
-        <f t="shared" si="103"/>
+        <f t="shared" si="108"/>
         <v>568.16284708702096</v>
       </c>
       <c r="N337" s="29">
-        <f t="shared" si="103"/>
+        <f t="shared" si="108"/>
         <v>630.33417867284697</v>
       </c>
       <c r="O337" s="29">
-        <f t="shared" si="103"/>
+        <f t="shared" si="108"/>
         <v>700.58234540278136</v>
       </c>
     </row>
     <row r="338" spans="1:15" hidden="1" outlineLevel="1">
+      <c r="B338" s="5"/>
       <c r="C338" s="6" t="s">
         <v>327</v>
       </c>
@@ -10330,19 +10660,19 @@
         <v>1502.6086145201625</v>
       </c>
       <c r="L338" s="31">
-        <f t="shared" ref="L338:O338" si="104">SUM(L334:L337)</f>
+        <f t="shared" ref="L338:O338" si="109">SUM(L334:L337)</f>
         <v>1545.6020050558077</v>
       </c>
       <c r="M338" s="31">
-        <f t="shared" si="104"/>
+        <f t="shared" si="109"/>
         <v>1575.0037492276851</v>
       </c>
       <c r="N338" s="31">
-        <f t="shared" si="104"/>
+        <f t="shared" si="109"/>
         <v>1731.9259221818411</v>
       </c>
       <c r="O338" s="31">
-        <f t="shared" si="104"/>
+        <f t="shared" si="109"/>
         <v>1904.6768308716623</v>
       </c>
     </row>
@@ -10362,19 +10692,19 @@
         <v>1167.4769021301263</v>
       </c>
       <c r="L340" s="29">
-        <f t="shared" ref="L340:O340" si="105">SUM(L338,L332)</f>
+        <f t="shared" ref="L340:O340" si="110">SUM(L338,L332)</f>
         <v>1180.1876091418103</v>
       </c>
       <c r="M340" s="29">
-        <f t="shared" si="105"/>
+        <f t="shared" si="110"/>
         <v>1167.4086632739532</v>
       </c>
       <c r="N340" s="29">
-        <f t="shared" si="105"/>
+        <f t="shared" si="110"/>
         <v>1279.7296635687121</v>
       </c>
       <c r="O340" s="29">
-        <f t="shared" si="105"/>
+        <f t="shared" si="110"/>
         <v>1402.085148300102</v>
       </c>
     </row>
@@ -10382,7 +10712,7 @@
     <row r="342" spans="1:15" collapsed="1"/>
     <row r="343" spans="1:15">
       <c r="A343" s="115" t="s">
-        <v>330</v>
+        <v>353</v>
       </c>
       <c r="B343" s="115"/>
       <c r="C343" s="115"/>
@@ -10399,32 +10729,33 @@
       <c r="N343" s="115"/>
       <c r="O343" s="115"/>
     </row>
-    <row r="345" spans="1:15">
+    <row r="344" spans="1:15" outlineLevel="1"/>
+    <row r="345" spans="1:15" outlineLevel="1">
       <c r="A345" s="2" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="B345" s="2"/>
       <c r="C345" s="2"/>
       <c r="D345" s="2"/>
       <c r="E345" s="4"/>
       <c r="F345" s="4">
-        <f t="shared" ref="F345:J345" si="106">G345-1</f>
+        <f t="shared" ref="F345:J345" si="111">G345-1</f>
         <v>2020</v>
       </c>
       <c r="G345" s="4">
-        <f t="shared" si="106"/>
+        <f t="shared" si="111"/>
         <v>2021</v>
       </c>
       <c r="H345" s="4">
-        <f t="shared" si="106"/>
+        <f t="shared" si="111"/>
         <v>2022</v>
       </c>
       <c r="I345" s="4">
-        <f t="shared" si="106"/>
+        <f t="shared" si="111"/>
         <v>2023</v>
       </c>
       <c r="J345" s="4">
-        <f t="shared" si="106"/>
+        <f t="shared" si="111"/>
         <v>2024</v>
       </c>
       <c r="K345" s="7">
@@ -10448,11 +10779,1077 @@
         <v>2029</v>
       </c>
     </row>
+    <row r="346" spans="1:15" outlineLevel="1">
+      <c r="A346" s="221"/>
+      <c r="B346" s="221"/>
+      <c r="C346" s="221"/>
+      <c r="D346" s="221"/>
+      <c r="E346" s="222"/>
+      <c r="F346" s="222"/>
+      <c r="G346" s="222"/>
+      <c r="H346" s="222"/>
+      <c r="I346" s="222"/>
+      <c r="J346" s="222"/>
+      <c r="K346" s="223"/>
+      <c r="L346" s="223"/>
+      <c r="M346" s="223"/>
+      <c r="N346" s="223"/>
+      <c r="O346" s="223"/>
+    </row>
+    <row r="347" spans="1:15" outlineLevel="1">
+      <c r="C347" t="s">
+        <v>359</v>
+      </c>
+      <c r="K347" s="8">
+        <f>K48</f>
+        <v>3</v>
+      </c>
+      <c r="L347" s="8">
+        <f t="shared" ref="L347:O347" si="112">L48</f>
+        <v>2</v>
+      </c>
+      <c r="M347" s="8">
+        <f t="shared" si="112"/>
+        <v>2</v>
+      </c>
+      <c r="N347" s="8">
+        <f t="shared" si="112"/>
+        <v>2</v>
+      </c>
+      <c r="O347" s="8">
+        <f t="shared" si="112"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="348" spans="1:15" outlineLevel="1">
+      <c r="C348" t="s">
+        <v>333</v>
+      </c>
+      <c r="D348" t="s">
+        <v>233</v>
+      </c>
+      <c r="F348" s="28">
+        <f>F217</f>
+        <v>13</v>
+      </c>
+      <c r="G348" s="28">
+        <f t="shared" ref="G348:O348" si="113">G217</f>
+        <v>20</v>
+      </c>
+      <c r="H348" s="28">
+        <f t="shared" si="113"/>
+        <v>23</v>
+      </c>
+      <c r="I348" s="28">
+        <f t="shared" si="113"/>
+        <v>23</v>
+      </c>
+      <c r="J348" s="28">
+        <f t="shared" si="113"/>
+        <v>29</v>
+      </c>
+      <c r="K348" s="29">
+        <f t="shared" si="113"/>
+        <v>26</v>
+      </c>
+      <c r="L348" s="29">
+        <f t="shared" si="113"/>
+        <v>27</v>
+      </c>
+      <c r="M348" s="29">
+        <f t="shared" si="113"/>
+        <v>27</v>
+      </c>
+      <c r="N348" s="29">
+        <f t="shared" si="113"/>
+        <v>27</v>
+      </c>
+      <c r="O348" s="29">
+        <f t="shared" si="113"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="349" spans="1:15" outlineLevel="1">
+      <c r="C349" t="s">
+        <v>334</v>
+      </c>
+      <c r="D349" t="s">
+        <v>209</v>
+      </c>
+      <c r="F349" s="28">
+        <f>-F108</f>
+        <v>2810</v>
+      </c>
+      <c r="G349" s="28">
+        <f t="shared" ref="G349:J349" si="114">-G108</f>
+        <v>3588</v>
+      </c>
+      <c r="H349" s="28">
+        <f t="shared" si="114"/>
+        <v>3891</v>
+      </c>
+      <c r="I349" s="28">
+        <f t="shared" si="114"/>
+        <v>4323</v>
+      </c>
+      <c r="J349" s="28">
+        <f t="shared" si="114"/>
+        <v>4710</v>
+      </c>
+      <c r="K349" s="29"/>
+      <c r="L349" s="29"/>
+      <c r="M349" s="29"/>
+      <c r="N349" s="29"/>
+      <c r="O349" s="29"/>
+    </row>
+    <row r="350" spans="1:15" outlineLevel="1">
+      <c r="C350" t="s">
+        <v>335</v>
+      </c>
+      <c r="D350" t="s">
+        <v>209</v>
+      </c>
+      <c r="F350" s="28">
+        <f>F349/F348</f>
+        <v>216.15384615384616</v>
+      </c>
+      <c r="G350" s="28">
+        <f t="shared" ref="G350:J350" si="115">G349/G348</f>
+        <v>179.4</v>
+      </c>
+      <c r="H350" s="28">
+        <f t="shared" si="115"/>
+        <v>169.17391304347825</v>
+      </c>
+      <c r="I350" s="28">
+        <f t="shared" si="115"/>
+        <v>187.95652173913044</v>
+      </c>
+      <c r="J350" s="28">
+        <f t="shared" si="115"/>
+        <v>162.41379310344828</v>
+      </c>
+      <c r="K350" s="29">
+        <f>K46</f>
+        <v>165.66206896551725</v>
+      </c>
+      <c r="L350" s="29">
+        <f>L46</f>
+        <v>168.97531034482759</v>
+      </c>
+      <c r="M350" s="29">
+        <f>M46</f>
+        <v>172.35481655172416</v>
+      </c>
+      <c r="N350" s="29">
+        <f>N46</f>
+        <v>175.80191288275864</v>
+      </c>
+      <c r="O350" s="29">
+        <f>O46</f>
+        <v>179.31795114041381</v>
+      </c>
+    </row>
+    <row r="351" spans="1:15" outlineLevel="1">
+      <c r="B351" s="5"/>
+      <c r="C351" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D351" s="5"/>
+      <c r="E351" s="5"/>
+      <c r="F351" s="30"/>
+      <c r="G351" s="30"/>
+      <c r="H351" s="158"/>
+      <c r="I351" s="158"/>
+      <c r="J351" s="215"/>
+      <c r="K351" s="31">
+        <f>K350*K348</f>
+        <v>4307.2137931034486</v>
+      </c>
+      <c r="L351" s="31">
+        <f t="shared" ref="L351:O351" si="116">L350*L348</f>
+        <v>4562.3333793103448</v>
+      </c>
+      <c r="M351" s="31">
+        <f t="shared" si="116"/>
+        <v>4653.5800468965526</v>
+      </c>
+      <c r="N351" s="31">
+        <f t="shared" si="116"/>
+        <v>4746.6516478344838</v>
+      </c>
+      <c r="O351" s="31">
+        <f t="shared" si="116"/>
+        <v>4841.584680791173</v>
+      </c>
+    </row>
+    <row r="352" spans="1:15" outlineLevel="1">
+      <c r="B352" s="178"/>
+      <c r="C352" s="173" t="s">
+        <v>359</v>
+      </c>
+      <c r="D352" s="178"/>
+      <c r="E352" s="178"/>
+      <c r="F352" s="214"/>
+      <c r="G352" s="214"/>
+      <c r="H352" s="112"/>
+      <c r="I352" s="112"/>
+      <c r="J352" s="224"/>
+      <c r="K352" s="212">
+        <f>K347*K350</f>
+        <v>496.98620689655172</v>
+      </c>
+      <c r="L352" s="212">
+        <f t="shared" ref="L352:O352" si="117">L347*L350</f>
+        <v>337.95062068965518</v>
+      </c>
+      <c r="M352" s="212">
+        <f t="shared" si="117"/>
+        <v>344.70963310344831</v>
+      </c>
+      <c r="N352" s="212">
+        <f t="shared" si="117"/>
+        <v>351.60382576551729</v>
+      </c>
+      <c r="O352" s="212">
+        <f t="shared" si="117"/>
+        <v>358.63590228082762</v>
+      </c>
+    </row>
+    <row r="353" spans="2:15" outlineLevel="1">
+      <c r="B353" s="5"/>
+      <c r="C353" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="D353" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E353" s="5"/>
+      <c r="F353" s="30"/>
+      <c r="G353" s="30"/>
+      <c r="H353" s="30"/>
+      <c r="I353" s="30"/>
+      <c r="J353" s="30"/>
+      <c r="K353" s="31">
+        <f>SUM(K351:K352)</f>
+        <v>4804.2000000000007</v>
+      </c>
+      <c r="L353" s="31">
+        <f t="shared" ref="L353:O353" si="118">SUM(L351:L352)</f>
+        <v>4900.2839999999997</v>
+      </c>
+      <c r="M353" s="31">
+        <f t="shared" si="118"/>
+        <v>4998.2896800000008</v>
+      </c>
+      <c r="N353" s="31">
+        <f t="shared" si="118"/>
+        <v>5098.2554736000011</v>
+      </c>
+      <c r="O353" s="31">
+        <f t="shared" si="118"/>
+        <v>5200.2205830720004</v>
+      </c>
+    </row>
+    <row r="354" spans="2:15" outlineLevel="1">
+      <c r="F354" s="28"/>
+      <c r="G354" s="28"/>
+      <c r="H354" s="28"/>
+      <c r="I354" s="28"/>
+      <c r="J354" s="28"/>
+      <c r="K354" s="29"/>
+      <c r="L354" s="29"/>
+      <c r="M354" s="29"/>
+      <c r="N354" s="29"/>
+      <c r="O354" s="29"/>
+    </row>
+    <row r="355" spans="2:15" outlineLevel="1">
+      <c r="C355" t="s">
+        <v>337</v>
+      </c>
+      <c r="F355" s="28">
+        <f>E360</f>
+        <v>32626</v>
+      </c>
+      <c r="G355" s="28">
+        <f t="shared" ref="G355:O355" si="119">F360</f>
+        <v>34703</v>
+      </c>
+      <c r="H355" s="28">
+        <f t="shared" si="119"/>
+        <v>37658</v>
+      </c>
+      <c r="I355" s="28">
+        <f t="shared" si="119"/>
+        <v>39932</v>
+      </c>
+      <c r="J355" s="28">
+        <f t="shared" si="119"/>
+        <v>43369</v>
+      </c>
+      <c r="K355" s="29">
+        <f t="shared" si="119"/>
+        <v>46950</v>
+      </c>
+      <c r="L355" s="29">
+        <f t="shared" si="119"/>
+        <v>50795</v>
+      </c>
+      <c r="M355" s="29">
+        <f t="shared" si="119"/>
+        <v>54736.084000000003</v>
+      </c>
+      <c r="N355" s="29">
+        <f t="shared" si="119"/>
+        <v>58775.173680000007</v>
+      </c>
+      <c r="O355" s="29">
+        <f t="shared" si="119"/>
+        <v>62914.229153600012</v>
+      </c>
+    </row>
+    <row r="356" spans="2:15" outlineLevel="1">
+      <c r="C356" t="s">
+        <v>334</v>
+      </c>
+      <c r="F356" s="28">
+        <f>F349</f>
+        <v>2810</v>
+      </c>
+      <c r="G356" s="28">
+        <f>G349</f>
+        <v>3588</v>
+      </c>
+      <c r="H356" s="28">
+        <f>H349</f>
+        <v>3891</v>
+      </c>
+      <c r="I356" s="28">
+        <f>I349</f>
+        <v>4323</v>
+      </c>
+      <c r="J356" s="28">
+        <f>J349</f>
+        <v>4710</v>
+      </c>
+      <c r="K356" s="29">
+        <f>K353</f>
+        <v>4804.2000000000007</v>
+      </c>
+      <c r="L356" s="29">
+        <f t="shared" ref="L356:O356" si="120">L353</f>
+        <v>4900.2839999999997</v>
+      </c>
+      <c r="M356" s="29">
+        <f t="shared" si="120"/>
+        <v>4998.2896800000008</v>
+      </c>
+      <c r="N356" s="29">
+        <f t="shared" si="120"/>
+        <v>5098.2554736000011</v>
+      </c>
+      <c r="O356" s="29">
+        <f t="shared" si="120"/>
+        <v>5200.2205830720004</v>
+      </c>
+    </row>
+    <row r="357" spans="2:15" outlineLevel="1">
+      <c r="B357" s="5"/>
+      <c r="C357" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="D357" s="5"/>
+      <c r="E357" s="5"/>
+      <c r="F357" s="30">
+        <f>SUM(F355:F356)</f>
+        <v>35436</v>
+      </c>
+      <c r="G357" s="30">
+        <f t="shared" ref="G357:O357" si="121">SUM(G355:G356)</f>
+        <v>38291</v>
+      </c>
+      <c r="H357" s="30">
+        <f t="shared" si="121"/>
+        <v>41549</v>
+      </c>
+      <c r="I357" s="30">
+        <f t="shared" si="121"/>
+        <v>44255</v>
+      </c>
+      <c r="J357" s="30">
+        <f t="shared" si="121"/>
+        <v>48079</v>
+      </c>
+      <c r="K357" s="31">
+        <f t="shared" si="121"/>
+        <v>51754.2</v>
+      </c>
+      <c r="L357" s="31">
+        <f t="shared" si="121"/>
+        <v>55695.284</v>
+      </c>
+      <c r="M357" s="31">
+        <f t="shared" si="121"/>
+        <v>59734.373680000004</v>
+      </c>
+      <c r="N357" s="31">
+        <f t="shared" si="121"/>
+        <v>63873.429153600009</v>
+      </c>
+      <c r="O357" s="31">
+        <f t="shared" si="121"/>
+        <v>68114.449736672017</v>
+      </c>
+    </row>
+    <row r="358" spans="2:15" outlineLevel="1">
+      <c r="C358" t="s">
+        <v>348</v>
+      </c>
+      <c r="F358" s="28"/>
+      <c r="G358" s="28"/>
+      <c r="H358" s="28"/>
+      <c r="I358" s="28"/>
+      <c r="J358" s="28"/>
+      <c r="K358" s="29">
+        <f>$J$364</f>
+        <v>959.2</v>
+      </c>
+      <c r="L358" s="29">
+        <f t="shared" ref="L358:O358" si="122">$J$364</f>
+        <v>959.2</v>
+      </c>
+      <c r="M358" s="29">
+        <f t="shared" si="122"/>
+        <v>959.2</v>
+      </c>
+      <c r="N358" s="29">
+        <f t="shared" si="122"/>
+        <v>959.2</v>
+      </c>
+      <c r="O358" s="29">
+        <f t="shared" si="122"/>
+        <v>959.2</v>
+      </c>
+    </row>
+    <row r="359" spans="2:15" outlineLevel="1">
+      <c r="F359" s="28"/>
+      <c r="G359" s="28"/>
+      <c r="H359" s="28"/>
+      <c r="I359" s="28"/>
+      <c r="J359" s="28"/>
+      <c r="K359" s="29"/>
+      <c r="L359" s="29"/>
+      <c r="M359" s="29"/>
+      <c r="N359" s="29"/>
+      <c r="O359" s="29"/>
+    </row>
+    <row r="360" spans="2:15" outlineLevel="1">
+      <c r="C360" t="s">
+        <v>337</v>
+      </c>
+      <c r="D360" t="s">
+        <v>209</v>
+      </c>
+      <c r="E360" s="216">
+        <v>32626</v>
+      </c>
+      <c r="F360" s="216">
+        <v>34703</v>
+      </c>
+      <c r="G360" s="216">
+        <v>37658</v>
+      </c>
+      <c r="H360" s="216">
+        <v>39932</v>
+      </c>
+      <c r="I360" s="216">
+        <v>43369</v>
+      </c>
+      <c r="J360" s="216">
+        <v>46950</v>
+      </c>
+      <c r="K360" s="29">
+        <f>K357-K358</f>
+        <v>50795</v>
+      </c>
+      <c r="L360" s="29">
+        <f t="shared" ref="L360:O360" si="123">L357-L358</f>
+        <v>54736.084000000003</v>
+      </c>
+      <c r="M360" s="29">
+        <f t="shared" si="123"/>
+        <v>58775.173680000007</v>
+      </c>
+      <c r="N360" s="29">
+        <f t="shared" si="123"/>
+        <v>62914.229153600012</v>
+      </c>
+      <c r="O360" s="29">
+        <f t="shared" si="123"/>
+        <v>67155.24973667202</v>
+      </c>
+    </row>
+    <row r="361" spans="2:15" outlineLevel="1">
+      <c r="B361" s="5"/>
+      <c r="C361" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="D361" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E361" s="5"/>
+      <c r="F361" s="30">
+        <f>F357-F360</f>
+        <v>733</v>
+      </c>
+      <c r="G361" s="30">
+        <f t="shared" ref="G361:J361" si="124">G357-G360</f>
+        <v>633</v>
+      </c>
+      <c r="H361" s="30">
+        <f t="shared" si="124"/>
+        <v>1617</v>
+      </c>
+      <c r="I361" s="30">
+        <f t="shared" si="124"/>
+        <v>886</v>
+      </c>
+      <c r="J361" s="30">
+        <f t="shared" si="124"/>
+        <v>1129</v>
+      </c>
+      <c r="K361" s="31"/>
+      <c r="L361" s="31"/>
+      <c r="M361" s="31"/>
+      <c r="N361" s="31"/>
+      <c r="O361" s="31"/>
+    </row>
+    <row r="362" spans="2:15" outlineLevel="1">
+      <c r="C362" t="s">
+        <v>349</v>
+      </c>
+      <c r="D362" t="s">
+        <v>209</v>
+      </c>
+      <c r="F362" s="216">
+        <v>0</v>
+      </c>
+      <c r="G362" s="216">
+        <v>-84</v>
+      </c>
+      <c r="H362" s="216">
+        <v>-118</v>
+      </c>
+      <c r="I362" s="216">
+        <v>0</v>
+      </c>
+      <c r="J362" s="216">
+        <v>0</v>
+      </c>
+      <c r="K362" s="29"/>
+      <c r="L362" s="29"/>
+      <c r="M362" s="29"/>
+      <c r="N362" s="29"/>
+      <c r="O362" s="29"/>
+    </row>
+    <row r="363" spans="2:15" outlineLevel="1">
+      <c r="B363" s="5"/>
+      <c r="C363" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="D363" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E363" s="5"/>
+      <c r="F363" s="30">
+        <f t="shared" ref="F363:G363" si="125">F361+F362</f>
+        <v>733</v>
+      </c>
+      <c r="G363" s="30">
+        <f t="shared" si="125"/>
+        <v>549</v>
+      </c>
+      <c r="H363" s="30">
+        <f>H361+H362</f>
+        <v>1499</v>
+      </c>
+      <c r="I363" s="30">
+        <f t="shared" ref="I363:J363" si="126">I361+I362</f>
+        <v>886</v>
+      </c>
+      <c r="J363" s="30">
+        <f t="shared" si="126"/>
+        <v>1129</v>
+      </c>
+      <c r="K363" s="31"/>
+      <c r="L363" s="31"/>
+      <c r="M363" s="31"/>
+      <c r="N363" s="31"/>
+      <c r="O363" s="31"/>
+    </row>
+    <row r="364" spans="2:15" outlineLevel="1">
+      <c r="B364" s="178"/>
+      <c r="C364" s="173" t="s">
+        <v>351</v>
+      </c>
+      <c r="D364" s="173" t="s">
+        <v>209</v>
+      </c>
+      <c r="E364" s="178"/>
+      <c r="F364" s="214"/>
+      <c r="G364" s="214"/>
+      <c r="H364" s="214"/>
+      <c r="I364" s="214"/>
+      <c r="J364" s="214">
+        <f>AVERAGE(F363:J363)</f>
+        <v>959.2</v>
+      </c>
+      <c r="K364" s="212"/>
+      <c r="L364" s="212"/>
+      <c r="M364" s="212"/>
+      <c r="N364" s="212"/>
+      <c r="O364" s="212"/>
+    </row>
+    <row r="365" spans="2:15" outlineLevel="1">
+      <c r="F365" s="28"/>
+      <c r="G365" s="28"/>
+      <c r="H365" s="28"/>
+      <c r="I365" s="28"/>
+      <c r="J365" s="28"/>
+      <c r="K365" s="29"/>
+      <c r="L365" s="29"/>
+      <c r="M365" s="29"/>
+      <c r="N365" s="29"/>
+      <c r="O365" s="29"/>
+    </row>
+    <row r="366" spans="2:15" outlineLevel="1">
+      <c r="C366" t="s">
+        <v>340</v>
+      </c>
+      <c r="D366" t="s">
+        <v>209</v>
+      </c>
+      <c r="F366" s="28">
+        <f>(E360+F360)/2</f>
+        <v>33664.5</v>
+      </c>
+      <c r="G366" s="28">
+        <f t="shared" ref="G366:O366" si="127">(F360+G360)/2</f>
+        <v>36180.5</v>
+      </c>
+      <c r="H366" s="28">
+        <f t="shared" si="127"/>
+        <v>38795</v>
+      </c>
+      <c r="I366" s="28">
+        <f t="shared" si="127"/>
+        <v>41650.5</v>
+      </c>
+      <c r="J366" s="28">
+        <f t="shared" si="127"/>
+        <v>45159.5</v>
+      </c>
+      <c r="K366" s="29">
+        <f t="shared" si="127"/>
+        <v>48872.5</v>
+      </c>
+      <c r="L366" s="29">
+        <f t="shared" si="127"/>
+        <v>52765.542000000001</v>
+      </c>
+      <c r="M366" s="29">
+        <f t="shared" si="127"/>
+        <v>56755.628840000005</v>
+      </c>
+      <c r="N366" s="29">
+        <f t="shared" si="127"/>
+        <v>60844.70141680001</v>
+      </c>
+      <c r="O366" s="29">
+        <f t="shared" si="127"/>
+        <v>65034.739445136016</v>
+      </c>
+    </row>
+    <row r="367" spans="2:15" outlineLevel="1">
+      <c r="C367" t="s">
+        <v>341</v>
+      </c>
+      <c r="D367" t="s">
+        <v>209</v>
+      </c>
+      <c r="F367" s="28">
+        <f>-F97</f>
+        <v>-1645</v>
+      </c>
+      <c r="G367" s="28">
+        <f>-G97</f>
+        <v>-1781</v>
+      </c>
+      <c r="H367" s="28">
+        <f>-H97</f>
+        <v>-1900</v>
+      </c>
+      <c r="I367" s="28">
+        <f>-I97</f>
+        <v>-2077</v>
+      </c>
+      <c r="J367" s="28">
+        <f>-J97</f>
+        <v>-2237</v>
+      </c>
+      <c r="K367" s="29"/>
+      <c r="L367" s="29"/>
+      <c r="M367" s="29"/>
+      <c r="N367" s="29"/>
+      <c r="O367" s="29"/>
+    </row>
+    <row r="368" spans="2:15" outlineLevel="1">
+      <c r="B368" s="5"/>
+      <c r="C368" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="D368" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E368" s="5"/>
+      <c r="F368" s="158">
+        <f>-F367/F366</f>
+        <v>4.8864530885651056E-2</v>
+      </c>
+      <c r="G368" s="158">
+        <f t="shared" ref="G368:J368" si="128">-G367/G366</f>
+        <v>4.9225411478558891E-2</v>
+      </c>
+      <c r="H368" s="158">
+        <f t="shared" si="128"/>
+        <v>4.8975383425699189E-2</v>
+      </c>
+      <c r="I368" s="158">
+        <f t="shared" si="128"/>
+        <v>4.9867348531230114E-2</v>
+      </c>
+      <c r="J368" s="158">
+        <f t="shared" si="128"/>
+        <v>4.953553515871522E-2</v>
+      </c>
+      <c r="K368" s="31"/>
+      <c r="L368" s="31"/>
+      <c r="M368" s="31"/>
+      <c r="N368" s="31"/>
+      <c r="O368" s="31"/>
+    </row>
+    <row r="369" spans="1:15" outlineLevel="1">
+      <c r="B369" s="178"/>
+      <c r="C369" s="173" t="s">
+        <v>352</v>
+      </c>
+      <c r="D369" s="178"/>
+      <c r="E369" s="178"/>
+      <c r="F369" s="112"/>
+      <c r="G369" s="112"/>
+      <c r="H369" s="112"/>
+      <c r="I369" s="112"/>
+      <c r="J369" s="112">
+        <f>AVERAGE(F368:J368)</f>
+        <v>4.9293641895970894E-2</v>
+      </c>
+      <c r="K369" s="212"/>
+      <c r="L369" s="212"/>
+      <c r="M369" s="212"/>
+      <c r="N369" s="212"/>
+      <c r="O369" s="212"/>
+    </row>
+    <row r="370" spans="1:15" outlineLevel="1">
+      <c r="F370" s="28"/>
+      <c r="G370" s="28"/>
+      <c r="H370" s="28"/>
+      <c r="I370" s="28"/>
+      <c r="J370" s="28"/>
+      <c r="K370" s="8"/>
+      <c r="L370" s="8"/>
+      <c r="M370" s="8"/>
+      <c r="N370" s="8"/>
+      <c r="O370" s="8"/>
+    </row>
+    <row r="371" spans="1:15" outlineLevel="1">
+      <c r="C371" t="s">
+        <v>343</v>
+      </c>
+      <c r="D371" t="s">
+        <v>209</v>
+      </c>
+      <c r="F371" s="28"/>
+      <c r="G371" s="28"/>
+      <c r="H371" s="28"/>
+      <c r="I371" s="28"/>
+      <c r="J371" s="28"/>
+      <c r="K371" s="29">
+        <f>-K366*$J$369</f>
+        <v>-2409.1035135608377</v>
+      </c>
+      <c r="L371" s="29">
+        <f>-L366*$J$369</f>
+        <v>-2601.0057317948117</v>
+      </c>
+      <c r="M371" s="29">
+        <f>-M366*$J$369</f>
+        <v>-2797.6916436195984</v>
+      </c>
+      <c r="N371" s="29">
+        <f>-N366*$J$369</f>
+        <v>-2999.2569229070127</v>
+      </c>
+      <c r="O371" s="29">
+        <f>-O366*$J$369</f>
+        <v>-3205.7991570063077</v>
+      </c>
+    </row>
+    <row r="372" spans="1:15" outlineLevel="1">
+      <c r="F372" s="28"/>
+      <c r="G372" s="28"/>
+      <c r="H372" s="28"/>
+      <c r="I372" s="28"/>
+      <c r="J372" s="28"/>
+      <c r="K372" s="29"/>
+      <c r="L372" s="29"/>
+      <c r="M372" s="29"/>
+      <c r="N372" s="29"/>
+      <c r="O372" s="29"/>
+    </row>
+    <row r="373" spans="1:15" outlineLevel="1">
+      <c r="C373" t="s">
+        <v>344</v>
+      </c>
+      <c r="D373" t="s">
+        <v>209</v>
+      </c>
+      <c r="F373" s="28"/>
+      <c r="G373" s="28"/>
+      <c r="H373" s="28"/>
+      <c r="I373" s="28"/>
+      <c r="J373" s="28"/>
+      <c r="K373" s="29">
+        <f>J376</f>
+        <v>29032</v>
+      </c>
+      <c r="L373" s="29">
+        <f t="shared" ref="L373:O373" si="129">K376</f>
+        <v>31427.096486439161</v>
+      </c>
+      <c r="M373" s="29">
+        <f t="shared" si="129"/>
+        <v>33726.374754644348</v>
+      </c>
+      <c r="N373" s="29">
+        <f t="shared" si="129"/>
+        <v>35926.972791024753</v>
+      </c>
+      <c r="O373" s="29">
+        <f t="shared" si="129"/>
+        <v>38025.971341717741</v>
+      </c>
+    </row>
+    <row r="374" spans="1:15" outlineLevel="1">
+      <c r="C374" t="s">
+        <v>345</v>
+      </c>
+      <c r="D374" t="s">
+        <v>209</v>
+      </c>
+      <c r="F374" s="28"/>
+      <c r="G374" s="28"/>
+      <c r="H374" s="28"/>
+      <c r="I374" s="28"/>
+      <c r="J374" s="28"/>
+      <c r="K374" s="29">
+        <f>K356</f>
+        <v>4804.2000000000007</v>
+      </c>
+      <c r="L374" s="29">
+        <f t="shared" ref="L374:O374" si="130">L356</f>
+        <v>4900.2839999999997</v>
+      </c>
+      <c r="M374" s="29">
+        <f t="shared" si="130"/>
+        <v>4998.2896800000008</v>
+      </c>
+      <c r="N374" s="29">
+        <f t="shared" si="130"/>
+        <v>5098.2554736000011</v>
+      </c>
+      <c r="O374" s="29">
+        <f t="shared" si="130"/>
+        <v>5200.2205830720004</v>
+      </c>
+    </row>
+    <row r="375" spans="1:15" outlineLevel="1">
+      <c r="C375" t="s">
+        <v>346</v>
+      </c>
+      <c r="D375" t="s">
+        <v>209</v>
+      </c>
+      <c r="F375" s="28"/>
+      <c r="G375" s="28"/>
+      <c r="H375" s="28"/>
+      <c r="I375" s="28"/>
+      <c r="J375" s="28"/>
+      <c r="K375" s="29">
+        <f>K371</f>
+        <v>-2409.1035135608377</v>
+      </c>
+      <c r="L375" s="29">
+        <f t="shared" ref="L375:O375" si="131">L371</f>
+        <v>-2601.0057317948117</v>
+      </c>
+      <c r="M375" s="29">
+        <f t="shared" si="131"/>
+        <v>-2797.6916436195984</v>
+      </c>
+      <c r="N375" s="29">
+        <f t="shared" si="131"/>
+        <v>-2999.2569229070127</v>
+      </c>
+      <c r="O375" s="29">
+        <f t="shared" si="131"/>
+        <v>-3205.7991570063077</v>
+      </c>
+    </row>
+    <row r="376" spans="1:15" outlineLevel="1">
+      <c r="B376" s="5"/>
+      <c r="C376" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D376" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E376" s="5"/>
+      <c r="F376" s="30"/>
+      <c r="G376" s="30"/>
+      <c r="H376" s="30"/>
+      <c r="I376" s="30"/>
+      <c r="J376" s="217">
+        <v>29032</v>
+      </c>
+      <c r="K376" s="31">
+        <f>SUM(K373:K375)</f>
+        <v>31427.096486439161</v>
+      </c>
+      <c r="L376" s="31">
+        <f t="shared" ref="L376:O376" si="132">SUM(L373:L375)</f>
+        <v>33726.374754644348</v>
+      </c>
+      <c r="M376" s="31">
+        <f t="shared" si="132"/>
+        <v>35926.972791024753</v>
+      </c>
+      <c r="N376" s="31">
+        <f t="shared" si="132"/>
+        <v>38025.971341717741</v>
+      </c>
+      <c r="O376" s="31">
+        <f t="shared" si="132"/>
+        <v>40020.392767783429</v>
+      </c>
+    </row>
+    <row r="377" spans="1:15" outlineLevel="1">
+      <c r="F377" s="28"/>
+      <c r="G377" s="28"/>
+      <c r="H377" s="28"/>
+      <c r="I377" s="28"/>
+      <c r="J377" s="28"/>
+      <c r="K377" s="28"/>
+      <c r="L377" s="28"/>
+      <c r="M377" s="28"/>
+      <c r="N377" s="28"/>
+      <c r="O377" s="28"/>
+    </row>
+    <row r="378" spans="1:15">
+      <c r="F378" s="28"/>
+      <c r="G378" s="28"/>
+      <c r="H378" s="28"/>
+      <c r="I378" s="28"/>
+      <c r="J378" s="28"/>
+      <c r="K378" s="28"/>
+      <c r="L378" s="28"/>
+      <c r="M378" s="28"/>
+      <c r="N378" s="28"/>
+      <c r="O378" s="28"/>
+    </row>
+    <row r="379" spans="1:15">
+      <c r="A379" s="115" t="s">
+        <v>355</v>
+      </c>
+      <c r="B379" s="115"/>
+      <c r="C379" s="115"/>
+      <c r="D379" s="115"/>
+      <c r="E379" s="115"/>
+      <c r="F379" s="115"/>
+      <c r="G379" s="115"/>
+      <c r="H379" s="115"/>
+      <c r="I379" s="115"/>
+      <c r="J379" s="115"/>
+      <c r="K379" s="115"/>
+      <c r="L379" s="115"/>
+      <c r="M379" s="115"/>
+      <c r="N379" s="115"/>
+      <c r="O379" s="115"/>
+    </row>
+    <row r="381" spans="1:15">
+      <c r="A381" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B381" s="2"/>
+      <c r="C381" s="2"/>
+      <c r="D381" s="2"/>
+      <c r="E381" s="4"/>
+      <c r="F381" s="4">
+        <f t="shared" ref="F381:J381" si="133">G381-1</f>
+        <v>2020</v>
+      </c>
+      <c r="G381" s="4">
+        <f t="shared" si="133"/>
+        <v>2021</v>
+      </c>
+      <c r="H381" s="4">
+        <f t="shared" si="133"/>
+        <v>2022</v>
+      </c>
+      <c r="I381" s="4">
+        <f t="shared" si="133"/>
+        <v>2023</v>
+      </c>
+      <c r="J381" s="4">
+        <f t="shared" si="133"/>
+        <v>2024</v>
+      </c>
+      <c r="K381" s="7">
+        <f>K$8</f>
+        <v>2025</v>
+      </c>
+      <c r="L381" s="7">
+        <f>L$8</f>
+        <v>2026</v>
+      </c>
+      <c r="M381" s="7">
+        <f>M$8</f>
+        <v>2027</v>
+      </c>
+      <c r="N381" s="7">
+        <f>N$8</f>
+        <v>2028</v>
+      </c>
+      <c r="O381" s="7">
+        <f>O$8</f>
+        <v>2029</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="A282:O282"/>
     <mergeCell ref="A307:O307"/>
     <mergeCell ref="A343:O343"/>
+    <mergeCell ref="A379:O379"/>
     <mergeCell ref="A187:O187"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
@@ -10561,17 +11958,17 @@
     </row>
     <row r="14" spans="7:7">
       <c r="G14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="7:7">
       <c r="G15" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" spans="7:7">
       <c r="G16" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>